<commit_message>
Fixed problems with GUI and added to README
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1379">
   <si>
     <t>Feature</t>
   </si>
@@ -2149,7 +2149,7 @@
     <t>{'Original': {}, 'Wavelet': {}}</t>
   </si>
   <si>
-    <t>9c3dc18795354a5aa591e55bfd48ef72397799ab</t>
+    <t>9faee00c7c4fd5780b7351656d5ddc4924cf1da8</t>
   </si>
   <si>
     <t>3D</t>
@@ -2158,1996 +2158,1999 @@
     <t>(1.0, 1.0, 1.0)</t>
   </si>
   <si>
-    <t>(246, 258, 213)</t>
-  </si>
-  <si>
-    <t>6402e994b53e95f677e4a93b60948c4835ced28d</t>
-  </si>
-  <si>
-    <t>(52, 66, 27, 156, 155, 116)</t>
-  </si>
-  <si>
-    <t>(121.66426908797446, 148.5435132339648, 91.18908684673764)</t>
-  </si>
-  <si>
-    <t>154.7804897265802</t>
-  </si>
-  <si>
-    <t>177.867928531256</t>
-  </si>
-  <si>
-    <t>171.18703221914913</t>
-  </si>
-  <si>
-    <t>178.9441253576099</t>
-  </si>
-  <si>
-    <t>567601.2916666666</t>
-  </si>
-  <si>
-    <t>0.4207225528547865</t>
-  </si>
-  <si>
-    <t>78798.37259489244</t>
-  </si>
-  <si>
-    <t>0.13882697899350113</t>
-  </si>
-  <si>
-    <t>-546.0000000000002</t>
-  </si>
-  <si>
-    <t>-271.0000000000015</t>
-  </si>
-  <si>
-    <t>111473581555.00002</t>
-  </si>
-  <si>
-    <t>3.913936071941399</t>
-  </si>
-  <si>
-    <t>145.00000000000023</t>
-  </si>
-  <si>
-    <t>2.448244841984789</t>
-  </si>
-  <si>
-    <t>-122.00000000000003</t>
-  </si>
-  <si>
-    <t>83.59210323295395</t>
-  </si>
-  <si>
-    <t>-431.5069486905238</t>
-  </si>
-  <si>
-    <t>-454.0000000000001</t>
-  </si>
-  <si>
-    <t>-844.0</t>
-  </si>
-  <si>
-    <t>722.0</t>
-  </si>
-  <si>
-    <t>61.21917587612843</t>
-  </si>
-  <si>
-    <t>443.19672218112436</t>
-  </si>
-  <si>
-    <t>0.5492361777671034</t>
-  </si>
-  <si>
-    <t>0.07546463702231947</t>
-  </si>
-  <si>
-    <t>10225.087783886376</t>
-  </si>
-  <si>
-    <t>298.5671020452069</t>
-  </si>
-  <si>
-    <t>7621.257291631253</t>
-  </si>
-  <si>
-    <t>220.18967746604477</t>
-  </si>
-  <si>
-    <t>54.675559326400325</t>
-  </si>
-  <si>
-    <t>4.204946574063089</t>
-  </si>
-  <si>
-    <t>0.8565761787253057</t>
-  </si>
-  <si>
-    <t>1.4478323402380144</t>
-  </si>
-  <si>
-    <t>2.24254320546298</t>
-  </si>
-  <si>
-    <t>2.04985620668348</t>
-  </si>
-  <si>
-    <t>0.5469166919129397</t>
-  </si>
-  <si>
-    <t>0.4976969134981242</t>
-  </si>
-  <si>
-    <t>0.9954393015247442</t>
-  </si>
-  <si>
-    <t>0.9558589446187978</t>
-  </si>
-  <si>
-    <t>-0.2683480166577544</t>
-  </si>
-  <si>
-    <t>0.9281344270457725</t>
-  </si>
-  <si>
-    <t>0.44385842724474067</t>
-  </si>
-  <si>
-    <t>16.909951936926102</t>
-  </si>
-  <si>
-    <t>0.015114909907859768</t>
-  </si>
-  <si>
-    <t>6.687834919002697</t>
-  </si>
-  <si>
-    <t>0.8682807973613562</t>
-  </si>
-  <si>
-    <t>0.0396929207187416</t>
-  </si>
-  <si>
-    <t>33.8199038738522</t>
-  </si>
-  <si>
-    <t>4.814335293031057</t>
-  </si>
-  <si>
-    <t>14.72012647511585</t>
-  </si>
-  <si>
-    <t>30528.935347182018</t>
-  </si>
-  <si>
-    <t>0.07120236608367542</t>
-  </si>
-  <si>
-    <t>17.046807819814717</t>
-  </si>
-  <si>
-    <t>327.4160274330909</t>
-  </si>
-  <si>
-    <t>2.3013445102432875</t>
-  </si>
-  <si>
-    <t>672.751012933431</t>
-  </si>
-  <si>
-    <t>0.009629520751034017</t>
-  </si>
-  <si>
-    <t>0.0038149512266145314</t>
-  </si>
-  <si>
-    <t>4.984129464827394</t>
-  </si>
-  <si>
-    <t>271082.88781618036</t>
-  </si>
-  <si>
-    <t>0.6302030492617491</t>
-  </si>
-  <si>
-    <t>0.7552927252196173</t>
-  </si>
-  <si>
-    <t>0.5334963150428891</t>
-  </si>
-  <si>
-    <t>0.821293854675566</t>
-  </si>
-  <si>
-    <t>278.39716670320036</t>
-  </si>
-  <si>
-    <t>0.0030330989402698317</t>
-  </si>
-  <si>
-    <t>2123.7337782591985</t>
-  </si>
-  <si>
-    <t>0.07420712737199757</t>
-  </si>
-  <si>
-    <t>17.533205358366413</t>
-  </si>
-  <si>
-    <t>452.29337153639193</t>
-  </si>
-  <si>
-    <t>388994.32604213984</t>
-  </si>
-  <si>
-    <t>98786535.17967086</t>
-  </si>
-  <si>
-    <t>1682.1167910165234</t>
-  </si>
-  <si>
-    <t>0.0028850557414384437</t>
-  </si>
-  <si>
-    <t>7725.329711031133</t>
-  </si>
-  <si>
-    <t>0.2699370946235415</t>
-  </si>
-  <si>
-    <t>0.5322671080643303</t>
-  </si>
-  <si>
-    <t>246.20314846264858</t>
-  </si>
-  <si>
-    <t>0.0014669317222836098</t>
-  </si>
-  <si>
-    <t>6.726754092483811</t>
-  </si>
-  <si>
-    <t>0.05042844531529452</t>
-  </si>
-  <si>
-    <t>388601.09405181615</t>
-  </si>
-  <si>
-    <t>-24.469417496403402</t>
-  </si>
-  <si>
-    <t>40.45289517018566</t>
-  </si>
-  <si>
-    <t>498637900.85518616</t>
-  </si>
-  <si>
-    <t>2.2133521716601363</t>
-  </si>
-  <si>
-    <t>32.080161678279545</t>
-  </si>
-  <si>
-    <t>6.613103544184021</t>
-  </si>
-  <si>
-    <t>282.8167891146416</t>
-  </si>
-  <si>
-    <t>21.047001407996234</t>
-  </si>
-  <si>
-    <t>7.531429460692879</t>
-  </si>
-  <si>
-    <t>5.553647511031629</t>
-  </si>
-  <si>
-    <t>-136.1848727939976</t>
-  </si>
-  <si>
-    <t>419.0016619086392</t>
-  </si>
-  <si>
-    <t>13.474650963257448</t>
-  </si>
-  <si>
-    <t>29.641706661407614</t>
-  </si>
-  <si>
-    <t>0.9020671578764872</t>
-  </si>
-  <si>
-    <t>0.2703673470920117</t>
-  </si>
-  <si>
-    <t>821.9083440795437</t>
-  </si>
-  <si>
-    <t>46.98542141562527</t>
-  </si>
-  <si>
-    <t>128.59705127871425</t>
-  </si>
-  <si>
-    <t>8.887699716727123</t>
-  </si>
-  <si>
-    <t>4.24989694688525</t>
-  </si>
-  <si>
-    <t>1.1480508470050277</t>
-  </si>
-  <si>
-    <t>0.5725030333500221</t>
-  </si>
-  <si>
-    <t>0.7537999578364434</t>
-  </si>
-  <si>
-    <t>1.4949251879647263</t>
-  </si>
-  <si>
-    <t>0.5498838852725502</t>
-  </si>
-  <si>
-    <t>0.6799311870708953</t>
-  </si>
-  <si>
-    <t>0.6616070686004284</t>
-  </si>
-  <si>
-    <t>0.9965050989658668</t>
-  </si>
-  <si>
-    <t>0.9613335948186637</t>
-  </si>
-  <si>
-    <t>-0.1488032540434546</t>
-  </si>
-  <si>
-    <t>0.6390013089374684</t>
-  </si>
-  <si>
-    <t>0.48626950929805385</t>
-  </si>
-  <si>
-    <t>6.797788678146111</t>
-  </si>
-  <si>
-    <t>0.09422615101902333</t>
-  </si>
-  <si>
-    <t>4.056138735570103</t>
-  </si>
-  <si>
-    <t>0.6750758396932217</t>
-  </si>
-  <si>
-    <t>0.18217187770465385</t>
-  </si>
-  <si>
-    <t>13.595577356292221</t>
-  </si>
-  <si>
-    <t>2.9760863533563415</t>
-  </si>
-  <si>
-    <t>1.3494869484725691</t>
-  </si>
-  <si>
-    <t>83086.86899520572</t>
-  </si>
-  <si>
-    <t>0.24051493431937462</t>
-  </si>
-  <si>
-    <t>1.6972803255443745</t>
-  </si>
-  <si>
-    <t>48.34225178872777</t>
-  </si>
-  <si>
-    <t>4.286454348766449</t>
-  </si>
-  <si>
-    <t>200.70869425764397</t>
-  </si>
-  <si>
-    <t>0.10031827663833538</t>
-  </si>
-  <si>
-    <t>0.023994982877888336</t>
-  </si>
-  <si>
-    <t>3.9197598847738884</t>
-  </si>
-  <si>
-    <t>160305.3305984844</t>
-  </si>
-  <si>
-    <t>0.4508695531347315</t>
-  </si>
-  <si>
-    <t>0.6087570945011339</t>
-  </si>
-  <si>
-    <t>1.3476571619894269</t>
-  </si>
-  <si>
-    <t>0.6861513151240489</t>
-  </si>
-  <si>
-    <t>33.5765132681236</t>
-  </si>
-  <si>
-    <t>0.016635868643390676</t>
-  </si>
-  <si>
-    <t>1470.7378435517971</t>
-  </si>
-  <si>
-    <t>0.18290484312296942</t>
-  </si>
-  <si>
-    <t>5.9667199632476775</t>
-  </si>
-  <si>
-    <t>51.65228205447084</t>
-  </si>
-  <si>
-    <t>10172876.563238403</t>
-  </si>
-  <si>
-    <t>460483275.43551797</t>
-  </si>
-  <si>
-    <t>232044.5262166039</t>
-  </si>
-  <si>
-    <t>0.03294712186484049</t>
-  </si>
-  <si>
-    <t>1377.4071632881482</t>
-  </si>
-  <si>
-    <t>0.1712979931958896</t>
-  </si>
-  <si>
-    <t>0.40760021656319856</t>
-  </si>
-  <si>
-    <t>21.025203297697402</t>
-  </si>
-  <si>
-    <t>0.013863881974660852</t>
-  </si>
-  <si>
-    <t>6.390660979475351</t>
-  </si>
-  <si>
-    <t>0.01416873855761149</t>
-  </si>
-  <si>
-    <t>10167895.32140746</t>
-  </si>
-  <si>
-    <t>-30.105116784767645</t>
-  </si>
-  <si>
-    <t>35.36007976737613</t>
-  </si>
-  <si>
-    <t>379648929.55148435</t>
-  </si>
-  <si>
-    <t>2.1423813026880647</t>
-  </si>
-  <si>
-    <t>34.068417632155146</t>
-  </si>
-  <si>
-    <t>3.1750658619061465</t>
-  </si>
-  <si>
-    <t>162.46878456039698</t>
-  </si>
-  <si>
-    <t>20.39743225773506</t>
-  </si>
-  <si>
-    <t>2.539673770124837</t>
-  </si>
-  <si>
-    <t>2.463530644808367</t>
-  </si>
-  <si>
-    <t>-138.19358496959356</t>
-  </si>
-  <si>
-    <t>300.66236952999054</t>
-  </si>
-  <si>
-    <t>14.159709155515298</t>
-  </si>
-  <si>
-    <t>25.864354977693594</t>
-  </si>
-  <si>
-    <t>0.021608673898172743</t>
-  </si>
-  <si>
-    <t>0.2659975923540755</t>
-  </si>
-  <si>
-    <t>662.5149155534833</t>
-  </si>
-  <si>
-    <t>43.836096831987874</t>
-  </si>
-  <si>
-    <t>24.90381695849899</t>
-  </si>
-  <si>
-    <t>0.09561182830980347</t>
-  </si>
-  <si>
-    <t>2.717823085408904</t>
-  </si>
-  <si>
-    <t>1.8058609420907246</t>
-  </si>
-  <si>
-    <t>0.20105186169915687</t>
-  </si>
-  <si>
-    <t>0.9879687162892599</t>
-  </si>
-  <si>
-    <t>1.7284612953363978</t>
-  </si>
-  <si>
-    <t>0.7741664713165017</t>
-  </si>
-  <si>
-    <t>0.6174178561789521</t>
-  </si>
-  <si>
-    <t>0.585207292860281</t>
-  </si>
-  <si>
-    <t>0.9896911771719379</t>
-  </si>
-  <si>
-    <t>0.933127099643994</t>
-  </si>
-  <si>
-    <t>-0.05602567917721112</t>
-  </si>
-  <si>
-    <t>0.2585899033003253</t>
-  </si>
-  <si>
-    <t>0.48944812059525256</t>
-  </si>
-  <si>
-    <t>6.603643124210724</t>
-  </si>
-  <si>
-    <t>0.07867819792937093</t>
-  </si>
-  <si>
-    <t>4.151092817322169</t>
-  </si>
-  <si>
-    <t>0.22920319317481408</t>
-  </si>
-  <si>
-    <t>0.1396928447503605</t>
-  </si>
-  <si>
-    <t>13.207286248421443</t>
-  </si>
-  <si>
-    <t>2.7470057853403165</t>
-  </si>
-  <si>
-    <t>1.130921006874907</t>
-  </si>
-  <si>
-    <t>94601.84126133169</t>
-  </si>
-  <si>
-    <t>0.24213892424035366</t>
-  </si>
-  <si>
-    <t>1.331945772798927</t>
-  </si>
-  <si>
-    <t>44.91377218502253</t>
-  </si>
-  <si>
-    <t>3.045286481425129</t>
-  </si>
-  <si>
-    <t>135.43859323032223</t>
-  </si>
-  <si>
-    <t>0.07475041081987302</t>
-  </si>
-  <si>
-    <t>0.02543591928259133</t>
-  </si>
-  <si>
-    <t>3.5027694862978414</t>
-  </si>
-  <si>
-    <t>216746.5120391413</t>
-  </si>
-  <si>
-    <t>0.5424672658632688</t>
-  </si>
-  <si>
-    <t>0.6893749438342816</t>
-  </si>
-  <si>
-    <t>0.8214759002236314</t>
-  </si>
-  <si>
-    <t>0.7577784670394644</t>
-  </si>
-  <si>
-    <t>34.15461736338553</t>
-  </si>
-  <si>
-    <t>0.01952092286790946</t>
-  </si>
-  <si>
-    <t>3167.144110359606</t>
-  </si>
-  <si>
-    <t>0.21209027726241253</t>
-  </si>
-  <si>
-    <t>5.257360875855547</t>
-  </si>
-  <si>
-    <t>48.67622045134936</t>
-  </si>
-  <si>
-    <t>5332862.746199692</t>
-  </si>
-  <si>
-    <t>237114419.07111767</t>
-  </si>
-  <si>
-    <t>124390.81984456678</t>
-  </si>
-  <si>
-    <t>0.034492044427770235</t>
-  </si>
-  <si>
-    <t>3061.533583338914</t>
-  </si>
-  <si>
-    <t>0.20501798589291595</t>
-  </si>
-  <si>
-    <t>0.4427891836907139</t>
-  </si>
-  <si>
-    <t>21.613603470117244</t>
-  </si>
-  <si>
-    <t>0.015849321409514054</t>
-  </si>
-  <si>
-    <t>5.474830198789418</t>
-  </si>
-  <si>
-    <t>0.02631286816077756</t>
-  </si>
-  <si>
-    <t>5331418.425549735</t>
-  </si>
-  <si>
-    <t>-11.393199447576242</t>
-  </si>
-  <si>
-    <t>11.25308871065548</t>
-  </si>
-  <si>
-    <t>45445085.88466932</t>
-  </si>
-  <si>
-    <t>1.0602334133347306</t>
-  </si>
-  <si>
-    <t>11.823720345130074</t>
-  </si>
-  <si>
-    <t>3.2243378543530175</t>
-  </si>
-  <si>
-    <t>49.782620482468424</t>
-  </si>
-  <si>
-    <t>7.079172201273348</t>
-  </si>
-  <si>
-    <t>-0.07044539735163666</t>
-  </si>
-  <si>
-    <t>-0.0593506635318935</t>
-  </si>
-  <si>
-    <t>-49.00288461191489</t>
-  </si>
-  <si>
-    <t>98.78550509438331</t>
-  </si>
-  <si>
-    <t>4.904427582686594</t>
-  </si>
-  <si>
-    <t>8.94857797133161</t>
-  </si>
-  <si>
-    <t>-0.010510217710087099</t>
-  </si>
-  <si>
-    <t>0.49304837387299627</t>
-  </si>
-  <si>
-    <t>80.07208515499336</t>
-  </si>
-  <si>
-    <t>6.241413556070139</t>
-  </si>
-  <si>
-    <t>0.6383761528899302</t>
-  </si>
-  <si>
-    <t>0.0007053062468939039</t>
-  </si>
-  <si>
-    <t>0.5428607459423284</t>
-  </si>
-  <si>
-    <t>0.5121028705245567</t>
-  </si>
-  <si>
-    <t>0.029155381639605328</t>
-  </si>
-  <si>
-    <t>0.498493789288889</t>
-  </si>
-  <si>
-    <t>1.0294745261262839</t>
-  </si>
-  <si>
-    <t>0.2561812682668235</t>
-  </si>
-  <si>
-    <t>0.7529994928630722</t>
-  </si>
-  <si>
-    <t>0.7521140134791223</t>
-  </si>
-  <si>
-    <t>0.9701219999001972</t>
-  </si>
-  <si>
-    <t>0.9007523875893052</t>
-  </si>
-  <si>
-    <t>-0.02292004716964298</t>
-  </si>
-  <si>
-    <t>0.1132515714776163</t>
-  </si>
-  <si>
-    <t>0.4867916631372766</t>
-  </si>
-  <si>
-    <t>2.4967426175552436</t>
-  </si>
-  <si>
-    <t>0.2504513400450726</t>
-  </si>
-  <si>
-    <t>2.0942108624109603</t>
-  </si>
-  <si>
-    <t>0.09744253527334196</t>
-  </si>
-  <si>
-    <t>0.27002424316186524</t>
-  </si>
-  <si>
-    <t>4.993485235110487</t>
-  </si>
-  <si>
-    <t>1.5523056074682702</t>
-  </si>
-  <si>
-    <t>0.2637409041167213</t>
-  </si>
-  <si>
-    <t>142229.96550859584</t>
-  </si>
-  <si>
-    <t>0.48671626066835477</t>
-  </si>
-  <si>
-    <t>0.2769398730266711</t>
-  </si>
-  <si>
-    <t>6.522435790168034</t>
-  </si>
-  <si>
-    <t>6.5106078943110886</t>
-  </si>
-  <si>
-    <t>42.19593807155457</t>
-  </si>
-  <si>
-    <t>1.1857560263376403</t>
-  </si>
-  <si>
-    <t>0.18558264357138016</t>
-  </si>
-  <si>
-    <t>3.0169939952325424</t>
-  </si>
-  <si>
-    <t>106041.10053244923</t>
-  </si>
-  <si>
-    <t>0.35271934374923813</t>
-  </si>
-  <si>
-    <t>0.5146297887925011</t>
-  </si>
-  <si>
-    <t>2.0583649994947657</t>
-  </si>
-  <si>
-    <t>0.573320048934848</t>
-  </si>
-  <si>
-    <t>3.7557832645491454</t>
-  </si>
-  <si>
-    <t>0.10813987229583481</t>
-  </si>
-  <si>
-    <t>1260.5681639085894</t>
-  </si>
-  <si>
-    <t>0.49667776355736387</t>
-  </si>
-  <si>
-    <t>2.2394961440323007</t>
-  </si>
-  <si>
-    <t>8.236012608353034</t>
-  </si>
-  <si>
-    <t>62563146.462174945</t>
-  </si>
-  <si>
-    <t>405106759.8317573</t>
-  </si>
-  <si>
-    <t>11339283.273306847</t>
-  </si>
-  <si>
-    <t>0.5460117327729621</t>
-  </si>
-  <si>
-    <t>1157.9621749408984</t>
-  </si>
-  <si>
-    <t>0.45624987192312777</t>
-  </si>
-  <si>
-    <t>0.6888398278020994</t>
-  </si>
-  <si>
-    <t>5.709515096037896</t>
-  </si>
-  <si>
-    <t>0.3739661453393012</t>
-  </si>
-  <si>
-    <t>2.5010842069186516</t>
-  </si>
-  <si>
-    <t>0.004472112729662724</t>
-  </si>
-  <si>
-    <t>62513145.942836575</t>
-  </si>
-  <si>
-    <t>-23.14517096244453</t>
-  </si>
-  <si>
-    <t>36.8178433776411</t>
-  </si>
-  <si>
-    <t>404649149.38660204</t>
-  </si>
-  <si>
-    <t>2.0993358592024376</t>
-  </si>
-  <si>
-    <t>29.8878745918395</t>
-  </si>
-  <si>
-    <t>5.851790623971707</t>
-  </si>
-  <si>
-    <t>224.62576866527397</t>
-  </si>
-  <si>
-    <t>19.30337740593943</t>
-  </si>
-  <si>
-    <t>6.311728429451349</t>
-  </si>
-  <si>
-    <t>4.775541322836342</t>
-  </si>
-  <si>
-    <t>-124.07981861589134</t>
-  </si>
-  <si>
-    <t>348.7055872811653</t>
-  </si>
-  <si>
-    <t>12.521554336884572</t>
-  </si>
-  <si>
-    <t>26.7023742316222</t>
-  </si>
-  <si>
-    <t>0.7033269811263023</t>
-  </si>
-  <si>
-    <t>0.28943797336538685</t>
-  </si>
-  <si>
-    <t>673.1788738384571</t>
-  </si>
-  <si>
-    <t>33.56294353020833</t>
-  </si>
-  <si>
-    <t>67.89005961633194</t>
-  </si>
-  <si>
-    <t>4.358436044860108</t>
-  </si>
-  <si>
-    <t>3.4085710022023785</t>
-  </si>
-  <si>
-    <t>1.011952820750842</t>
-  </si>
-  <si>
-    <t>0.5392261825732104</t>
-  </si>
-  <si>
-    <t>0.7039290694629806</t>
-  </si>
-  <si>
-    <t>1.4291801848213814</t>
-  </si>
-  <si>
-    <t>0.4906631335058341</t>
-  </si>
-  <si>
-    <t>0.693845138513121</t>
-  </si>
-  <si>
-    <t>0.6783964138066009</t>
-  </si>
-  <si>
-    <t>0.9949334828695414</t>
-  </si>
-  <si>
-    <t>0.9543193722180215</t>
-  </si>
-  <si>
-    <t>-0.1429388833249088</t>
-  </si>
-  <si>
-    <t>0.6120872706986927</t>
-  </si>
-  <si>
-    <t>0.48352823545174106</t>
-  </si>
-  <si>
-    <t>5.741406243592949</t>
-  </si>
-  <si>
-    <t>0.10620799339406917</t>
-  </si>
-  <si>
-    <t>3.8488679641223866</t>
-  </si>
-  <si>
-    <t>0.600130388097065</t>
-  </si>
-  <si>
-    <t>0.19675937681326167</t>
-  </si>
-  <si>
-    <t>11.482812487185896</t>
-  </si>
-  <si>
-    <t>2.850904475767774</t>
-  </si>
-  <si>
-    <t>1.105130955738305</t>
-  </si>
-  <si>
-    <t>85898.37428774446</t>
-  </si>
-  <si>
-    <t>0.25649180074201994</t>
-  </si>
-  <si>
-    <t>1.4240009154426756</t>
-  </si>
-  <si>
-    <t>34.84084165654495</t>
-  </si>
-  <si>
-    <t>4.632057613307134</t>
-  </si>
-  <si>
-    <t>155.70092856252475</t>
-  </si>
-  <si>
-    <t>0.15397237647320566</t>
-  </si>
-  <si>
-    <t>0.03451703455630185</t>
-  </si>
-  <si>
-    <t>3.878890360755622</t>
-  </si>
-  <si>
-    <t>148716.69395969552</t>
-  </si>
-  <si>
-    <t>0.4305375074221051</t>
-  </si>
-  <si>
-    <t>0.5902249488697119</t>
-  </si>
-  <si>
-    <t>1.4850134836440398</t>
-  </si>
-  <si>
-    <t>0.6678463234037099</t>
-  </si>
-  <si>
-    <t>23.63361992454261</t>
-  </si>
-  <si>
-    <t>0.02341394387985921</t>
-  </si>
-  <si>
-    <t>1549.2621664050234</t>
-  </si>
-  <si>
-    <t>0.202676892517664</t>
-  </si>
-  <si>
-    <t>5.369228328734384</t>
-  </si>
-  <si>
-    <t>39.70447409733124</t>
-  </si>
-  <si>
-    <t>11268565.65607012</t>
-  </si>
-  <si>
-    <t>361148191.4093407</t>
-  </si>
-  <si>
-    <t>364858.2122760082</t>
-  </si>
-  <si>
-    <t>0.050375518717408724</t>
-  </si>
-  <si>
-    <t>1233.330193615908</t>
-  </si>
-  <si>
-    <t>0.16134617917528885</t>
-  </si>
-  <si>
-    <t>0.39135332880377577</t>
-  </si>
-  <si>
-    <t>15.57785449159043</t>
-  </si>
-  <si>
-    <t>0.01991194933555855</t>
-  </si>
-  <si>
-    <t>6.330038624292325</t>
-  </si>
-  <si>
-    <t>0.013469200041584658</t>
-  </si>
-  <si>
-    <t>11263053.564877415</t>
-  </si>
-  <si>
-    <t>-9.053734463558062</t>
-  </si>
-  <si>
-    <t>8.76737839659415</t>
-  </si>
-  <si>
-    <t>27681982.303973958</t>
-  </si>
-  <si>
-    <t>1.0083385789122565</t>
-  </si>
-  <si>
-    <t>9.32482261900498</t>
-  </si>
-  <si>
-    <t>3.1262404630786236</t>
-  </si>
-  <si>
-    <t>35.480391345440495</t>
-  </si>
-  <si>
-    <t>5.549320364371384</t>
-  </si>
-  <si>
-    <t>-0.12244104566795798</t>
-  </si>
-  <si>
-    <t>-0.08416580548612113</t>
-  </si>
-  <si>
-    <t>-43.52691989054823</t>
-  </si>
-  <si>
-    <t>79.00731123598872</t>
-  </si>
-  <si>
-    <t>3.867703994844657</t>
-  </si>
-  <si>
-    <t>6.9840791999404095</t>
-  </si>
-  <si>
-    <t>-0.047887331929428865</t>
-  </si>
-  <si>
-    <t>0.49933131674648956</t>
-  </si>
-  <si>
-    <t>48.76237046137598</t>
-  </si>
-  <si>
-    <t>6.242160162254223</t>
-  </si>
-  <si>
-    <t>0.5429065764513696</t>
-  </si>
-  <si>
-    <t>0.0030185089622155672</t>
-  </si>
-  <si>
-    <t>0.5319592914217215</t>
-  </si>
-  <si>
-    <t>0.47303540436189545</t>
-  </si>
-  <si>
-    <t>0.058618848379698156</t>
-  </si>
-  <si>
-    <t>0.4720965095897487</t>
-  </si>
-  <si>
-    <t>0.9787609964349266</t>
-  </si>
-  <si>
-    <t>0.24208111385597716</t>
-  </si>
-  <si>
-    <t>0.7641075563704878</t>
-  </si>
-  <si>
-    <t>0.7640456346823403</t>
-  </si>
-  <si>
-    <t>0.9721911272983135</t>
-  </si>
-  <si>
-    <t>0.9056119178548367</t>
-  </si>
-  <si>
-    <t>-0.02684385231678986</t>
-  </si>
-  <si>
-    <t>0.17331240984881088</t>
-  </si>
-  <si>
-    <t>0.4712813166881545</t>
-  </si>
-  <si>
-    <t>2.495481708224502</t>
-  </si>
-  <si>
-    <t>0.25827686304367115</t>
-  </si>
-  <si>
-    <t>1.9880109364844563</t>
-  </si>
-  <si>
-    <t>0.1479769263469424</t>
-  </si>
-  <si>
-    <t>0.28848698076771223</t>
-  </si>
-  <si>
-    <t>4.990963416449004</t>
-  </si>
-  <si>
-    <t>1.5112137818379447</t>
-  </si>
-  <si>
-    <t>0.2512486739459042</t>
-  </si>
-  <si>
-    <t>140209.8343223958</t>
-  </si>
-  <si>
-    <t>0.49858516069136627</t>
-  </si>
-  <si>
-    <t>0.2528415426082886</t>
-  </si>
-  <si>
-    <t>6.490634096816289</t>
-  </si>
-  <si>
-    <t>7.391834922033824</t>
-  </si>
-  <si>
-    <t>47.76390586412002</t>
-  </si>
-  <si>
-    <t>1.3433992928594256</t>
-  </si>
-  <si>
-    <t>0.18153862692041706</t>
-  </si>
-  <si>
-    <t>3.0453969303770703</t>
-  </si>
-  <si>
-    <t>95900.34942240696</t>
-  </si>
-  <si>
-    <t>0.32990085740517944</t>
-  </si>
-  <si>
-    <t>0.4954794305721239</t>
-  </si>
-  <si>
-    <t>2.555714872128635</t>
-  </si>
-  <si>
-    <t>0.5663580132684742</t>
-  </si>
-  <si>
-    <t>3.6856138687772533</t>
-  </si>
-  <si>
-    <t>0.1028326347918713</t>
-  </si>
-  <si>
-    <t>136.54225352112675</t>
-  </si>
-  <si>
-    <t>0.4807825828208689</t>
-  </si>
-  <si>
-    <t>1.9376611783376316</t>
-  </si>
-  <si>
-    <t>6.253521126760563</t>
-  </si>
-  <si>
-    <t>566216219.0105634</t>
-  </si>
-  <si>
-    <t>3653608793.4859157</t>
-  </si>
-  <si>
-    <t>102977836.88930458</t>
-  </si>
-  <si>
-    <t>0.6425811815336463</t>
-  </si>
-  <si>
-    <t>157.09859154929578</t>
-  </si>
-  <si>
-    <t>0.5531640547510415</t>
-  </si>
-  <si>
-    <t>0.7718661129032561</t>
-  </si>
-  <si>
-    <t>4.920964073684298</t>
-  </si>
-  <si>
-    <t>0.4949757210037275</t>
-  </si>
-  <si>
-    <t>2.5989169233510743</t>
-  </si>
-  <si>
-    <t>0.0005004255379134017</t>
-  </si>
-  <si>
-    <t>562223018.9350699</t>
-  </si>
-  <si>
-    <t>-10.887209257138098</t>
-  </si>
-  <si>
-    <t>10.829238744463051</t>
-  </si>
-  <si>
-    <t>41558896.85109001</t>
-  </si>
-  <si>
-    <t>1.0428530098421103</t>
-  </si>
-  <si>
-    <t>11.362918130299725</t>
-  </si>
-  <si>
-    <t>3.162934834179758</t>
-  </si>
-  <si>
-    <t>47.91926696755102</t>
-  </si>
-  <si>
-    <t>6.786609576973931</t>
-  </si>
-  <si>
-    <t>-0.02535813604761159</t>
-  </si>
-  <si>
-    <t>-0.034885759483577417</t>
-  </si>
-  <si>
-    <t>-45.64324726788343</t>
-  </si>
-  <si>
-    <t>93.56251423543445</t>
-  </si>
-  <si>
-    <t>4.715315265538868</t>
-  </si>
-  <si>
-    <t>8.557414483777388</t>
-  </si>
-  <si>
-    <t>-0.0013483361989839464</t>
-  </si>
-  <si>
-    <t>0.49535937609867636</t>
-  </si>
-  <si>
-    <t>73.22869961209923</t>
-  </si>
-  <si>
-    <t>6.248909695831662</t>
-  </si>
-  <si>
-    <t>0.5897945576862341</t>
-  </si>
-  <si>
-    <t>0.0015777543273998934</t>
-  </si>
-  <si>
-    <t>0.5297231823542324</t>
-  </si>
-  <si>
-    <t>0.5073891339981981</t>
-  </si>
-  <si>
-    <t>0.02153882258321033</t>
-  </si>
-  <si>
-    <t>0.4977526386135972</t>
-  </si>
-  <si>
-    <t>1.0163556591183336</t>
-  </si>
-  <si>
-    <t>0.25205584918456647</t>
-  </si>
-  <si>
-    <t>0.7527170332750561</t>
-  </si>
-  <si>
-    <t>0.7520873302316615</t>
-  </si>
-  <si>
-    <t>0.9703268710670871</t>
-  </si>
-  <si>
-    <t>0.9007692339349869</t>
-  </si>
-  <si>
-    <t>-0.023197823830075865</t>
-  </si>
-  <si>
-    <t>0.11590829112738422</t>
-  </si>
-  <si>
-    <t>0.4894409327621662</t>
-  </si>
-  <si>
-    <t>2.4986647786089735</t>
-  </si>
-  <si>
-    <t>0.25279707308564</t>
-  </si>
-  <si>
-    <t>2.061092073055771</t>
-  </si>
-  <si>
-    <t>0.09952642640585631</t>
-  </si>
-  <si>
-    <t>0.27158933213622</t>
-  </si>
-  <si>
-    <t>4.997329557217947</t>
-  </si>
-  <si>
-    <t>1.5302803120709676</t>
-  </si>
-  <si>
-    <t>0.2592780790881076</t>
-  </si>
-  <si>
-    <t>143811.88306296227</t>
-  </si>
-  <si>
-    <t>0.4910503885929515</t>
-  </si>
-  <si>
-    <t>0.26807164526471366</t>
-  </si>
-  <si>
-    <t>6.514679137851474</t>
-  </si>
-  <si>
-    <t>6.5074502030925805</t>
-  </si>
-  <si>
-    <t>42.25536386234373</t>
-  </si>
-  <si>
-    <t>1.180397159955794</t>
-  </si>
-  <si>
-    <t>0.18381891221071278</t>
-  </si>
-  <si>
-    <t>2.9873721903938386</t>
-  </si>
-  <si>
-    <t>106589.78318759546</t>
-  </si>
-  <si>
-    <t>0.35359911814914236</t>
-  </si>
-  <si>
-    <t>0.5158239244883346</t>
-  </si>
-  <si>
-    <t>2.073725455232859</t>
-  </si>
-  <si>
-    <t>0.5734679782852679</t>
-  </si>
-  <si>
-    <t>3.746658545552861</t>
-  </si>
-  <si>
-    <t>0.10656726923543232</t>
-  </si>
-  <si>
-    <t>911.5831978319783</t>
-  </si>
-  <si>
-    <t>0.4940830340552728</t>
-  </si>
-  <si>
-    <t>2.238074044697086</t>
-  </si>
-  <si>
-    <t>8.48130081300813</t>
-  </si>
-  <si>
-    <t>86468292.6411924</t>
-  </si>
-  <si>
-    <t>560626404.9436314</t>
-  </si>
-  <si>
-    <t>15651706.605047425</t>
-  </si>
-  <si>
-    <t>0.5299119241192412</t>
-  </si>
-  <si>
-    <t>942.5967479674797</t>
-  </si>
-  <si>
-    <t>0.5108925463238372</t>
-  </si>
-  <si>
-    <t>0.7331245060806753</t>
-  </si>
-  <si>
-    <t>6.219356439233415</t>
-  </si>
-  <si>
-    <t>0.38847255166181444</t>
-  </si>
-  <si>
-    <t>2.3077033850876854</t>
-  </si>
-  <si>
-    <t>0.003251003934683895</t>
-  </si>
-  <si>
-    <t>86373676.54839376</t>
-  </si>
-  <si>
-    <t>-4.345477322112237</t>
-  </si>
-  <si>
-    <t>4.3636072901966765</t>
-  </si>
-  <si>
-    <t>6664734.274798911</t>
-  </si>
-  <si>
-    <t>0.9999990035888915</t>
-  </si>
-  <si>
-    <t>4.553858786875148</t>
-  </si>
-  <si>
-    <t>3.147028662361883</t>
-  </si>
-  <si>
-    <t>17.131641560993565</t>
-  </si>
-  <si>
-    <t>2.7187754217223774</t>
-  </si>
-  <si>
-    <t>0.0025874860704164443</t>
-  </si>
-  <si>
-    <t>-0.00441069255421625</t>
-  </si>
-  <si>
-    <t>-17.530363018640358</t>
-  </si>
-  <si>
-    <t>34.66200457963392</t>
-  </si>
-  <si>
-    <t>1.8899075267158185</t>
-  </si>
-  <si>
-    <t>3.4269043407968494</t>
-  </si>
-  <si>
-    <t>0.006341008356043798</t>
-  </si>
-  <si>
-    <t>0.5000006906593912</t>
-  </si>
-  <si>
-    <t>11.74366666588812</t>
-  </si>
-  <si>
-    <t>2.245339907622006</t>
-  </si>
-  <si>
-    <t>0.4943281863088314</t>
-  </si>
-  <si>
-    <t>0.0005954450448445639</t>
-  </si>
-  <si>
-    <t>0.4943282212642399</t>
-  </si>
-  <si>
-    <t>0.5056700631247932</t>
-  </si>
-  <si>
-    <t>-0.011341853512379728</t>
-  </si>
-  <si>
-    <t>0.9942920188480451</t>
-  </si>
-  <si>
-    <t>0.24802894194787364</t>
-  </si>
-  <si>
-    <t>0.7471649684376034</t>
-  </si>
-  <si>
-    <t>0.8988659873750412</t>
-  </si>
-  <si>
-    <t>0.8314433122917357</t>
-  </si>
-  <si>
-    <t>-0.005708021586134553</t>
-  </si>
-  <si>
-    <t>0.08650971572055279</t>
-  </si>
-  <si>
-    <t>1.4993916463948005</t>
-  </si>
-  <si>
-    <t>0.25197191585760986</t>
-  </si>
-  <si>
-    <t>1.9942895093797617</t>
-  </si>
-  <si>
-    <t>0.07232577230981117</t>
-  </si>
-  <si>
-    <t>0.2683747806900244</t>
-  </si>
-  <si>
-    <t>2.998783292789601</t>
-  </si>
-  <si>
-    <t>1.4886194462549691</t>
-  </si>
-  <si>
-    <t>0.24999957109725826</t>
-  </si>
-  <si>
-    <t>149884.6877289351</t>
-  </si>
-  <si>
-    <t>0.5000003607744214</t>
-  </si>
-  <si>
-    <t>0.24999981961278933</t>
-  </si>
-  <si>
-    <t>2.4999742603105046</t>
-  </si>
-  <si>
-    <t>5.40611297197457</t>
-  </si>
-  <si>
-    <t>13.492429493911338</t>
-  </si>
-  <si>
-    <t>3.38453384149038</t>
-  </si>
-  <si>
-    <t>0.6250064349223738</t>
-  </si>
-  <si>
-    <t>2.8691189404186708</t>
-  </si>
-  <si>
-    <t>107980.10878502694</t>
-  </si>
-  <si>
-    <t>0.35918645247174036</t>
-  </si>
-  <si>
-    <t>0.5282117607862916</t>
-  </si>
-  <si>
-    <t>1.7568077616438595</t>
-  </si>
-  <si>
-    <t>0.6029923743136215</t>
-  </si>
-  <si>
-    <t>1.5081882389086105</t>
-  </si>
-  <si>
-    <t>0.37669340816487407</t>
+    <t>(346, 242, 301)</t>
+  </si>
+  <si>
+    <t>821131876cef4de74aacc045755dcd2b8da100fd</t>
+  </si>
+  <si>
+    <t>(68, 66, 84, 188, 164, 142)</t>
+  </si>
+  <si>
+    <t>(152.2450767962042, 146.84154618051787, 157.2812907860725)</t>
+  </si>
+  <si>
+    <t>184.43969204051496</t>
+  </si>
+  <si>
+    <t>191.03141102970474</t>
+  </si>
+  <si>
+    <t>189.40168953839878</t>
+  </si>
+  <si>
+    <t>202.842303280159</t>
+  </si>
+  <si>
+    <t>863883.5833333334</t>
+  </si>
+  <si>
+    <t>0.39203651457255057</t>
+  </si>
+  <si>
+    <t>111890.8103334799</t>
+  </si>
+  <si>
+    <t>0.12952070451639353</t>
+  </si>
+  <si>
+    <t>-537.0</t>
+  </si>
+  <si>
+    <t>-254.00000000000006</t>
+  </si>
+  <si>
+    <t>162549139315.00003</t>
+  </si>
+  <si>
+    <t>3.893939865364668</t>
+  </si>
+  <si>
+    <t>158.00000000000068</t>
+  </si>
+  <si>
+    <t>2.257824808369796</t>
+  </si>
+  <si>
+    <t>-118.00000000000009</t>
+  </si>
+  <si>
+    <t>87.4462321047329</t>
+  </si>
+  <si>
+    <t>-420.65937666753683</t>
+  </si>
+  <si>
+    <t>-447.00000000000006</t>
+  </si>
+  <si>
+    <t>-838.0000000000001</t>
+  </si>
+  <si>
+    <t>720.0</t>
+  </si>
+  <si>
+    <t>66.14084993713128</t>
+  </si>
+  <si>
+    <t>433.29536963181255</t>
+  </si>
+  <si>
+    <t>0.5189906167395711</t>
+  </si>
+  <si>
+    <t>0.07604609640630673</t>
+  </si>
+  <si>
+    <t>10790.566166048438</t>
+  </si>
+  <si>
+    <t>315.3227367024196</t>
+  </si>
+  <si>
+    <t>8402.224183916971</t>
+  </si>
+  <si>
+    <t>254.55526148933117</t>
+  </si>
+  <si>
+    <t>59.27538007679528</t>
+  </si>
+  <si>
+    <t>3.68876325784467</t>
+  </si>
+  <si>
+    <t>0.8823396296875821</t>
+  </si>
+  <si>
+    <t>1.377913110284685</t>
+  </si>
+  <si>
+    <t>2.169965664242894</t>
+  </si>
+  <si>
+    <t>1.7338919181561292</t>
+  </si>
+  <si>
+    <t>0.5528326885853869</t>
+  </si>
+  <si>
+    <t>0.5048024301598444</t>
+  </si>
+  <si>
+    <t>0.9959814582209995</t>
+  </si>
+  <si>
+    <t>0.9577246837345754</t>
+  </si>
+  <si>
+    <t>-0.28278682002777783</t>
+  </si>
+  <si>
+    <t>0.9355965510282218</t>
+  </si>
+  <si>
+    <t>0.45175772815511694</t>
+  </si>
+  <si>
+    <t>17.361545157214948</t>
+  </si>
+  <si>
+    <t>0.015433981536710729</t>
+  </si>
+  <si>
+    <t>6.620273088131875</t>
+  </si>
+  <si>
+    <t>0.8869347560388481</t>
+  </si>
+  <si>
+    <t>0.041338683800445954</t>
+  </si>
+  <si>
+    <t>34.7230903144299</t>
+  </si>
+  <si>
+    <t>4.805841717279811</t>
+  </si>
+  <si>
+    <t>15.741035833659993</t>
+  </si>
+  <si>
+    <t>46847.48599428215</t>
+  </si>
+  <si>
+    <t>0.07198286731163125</t>
+  </si>
+  <si>
+    <t>17.58782383119823</t>
+  </si>
+  <si>
+    <t>340.82138553882845</t>
+  </si>
+  <si>
+    <t>2.322681856456085</t>
+  </si>
+  <si>
+    <t>725.5096094085098</t>
+  </si>
+  <si>
+    <t>0.009169590899442841</t>
+  </si>
+  <si>
+    <t>0.003665494088375261</t>
+  </si>
+  <si>
+    <t>4.9842665050792325</t>
+  </si>
+  <si>
+    <t>406743.21605096</t>
+  </si>
+  <si>
+    <t>0.6226898616374453</t>
+  </si>
+  <si>
+    <t>0.7515503260931177</t>
+  </si>
+  <si>
+    <t>0.53616889375732</t>
+  </si>
+  <si>
+    <t>0.8166260394092523</t>
+  </si>
+  <si>
+    <t>285.95490563779845</t>
+  </si>
+  <si>
+    <t>0.0029164168819911</t>
+  </si>
+  <si>
+    <t>2143.31230042151</t>
+  </si>
+  <si>
+    <t>0.06844144528105472</t>
+  </si>
+  <si>
+    <t>20.321182938425462</t>
+  </si>
+  <si>
+    <t>446.2408353557287</t>
+  </si>
+  <si>
+    <t>1086679.495082386</t>
+  </si>
+  <si>
+    <t>304940364.58359945</t>
+  </si>
+  <si>
+    <t>4345.977303477993</t>
+  </si>
+  <si>
+    <t>0.00306169451426477</t>
+  </si>
+  <si>
+    <t>7962.215991825265</t>
+  </si>
+  <si>
+    <t>0.2542539274436475</t>
+  </si>
+  <si>
+    <t>0.5156888922957006</t>
+  </si>
+  <si>
+    <t>235.85752167249734</t>
+  </si>
+  <si>
+    <t>0.0015626271164545593</t>
+  </si>
+  <si>
+    <t>6.9479861995334815</t>
+  </si>
+  <si>
+    <t>0.036170099723030084</t>
+  </si>
+  <si>
+    <t>1085915.1304430575</t>
+  </si>
+  <si>
+    <t>-25.04950227771793</t>
+  </si>
+  <si>
+    <t>33.21095509232845</t>
+  </si>
+  <si>
+    <t>509866262.0280064</t>
+  </si>
+  <si>
+    <t>2.029341210520733</t>
+  </si>
+  <si>
+    <t>29.948727249002605</t>
+  </si>
+  <si>
+    <t>4.54980253760124</t>
+  </si>
+  <si>
+    <t>216.97420635997392</t>
+  </si>
+  <si>
+    <t>18.45304042341233</t>
+  </si>
+  <si>
+    <t>3.9892817366007547</t>
+  </si>
+  <si>
+    <t>3.4693682184284973</t>
+  </si>
+  <si>
+    <t>-124.96386029826597</t>
+  </si>
+  <si>
+    <t>341.9380666582399</t>
+  </si>
+  <si>
+    <t>12.467890385976078</t>
+  </si>
+  <si>
+    <t>24.267210014606388</t>
+  </si>
+  <si>
+    <t>0.31418902126730597</t>
+  </si>
+  <si>
+    <t>0.29494081621716467</t>
+  </si>
+  <si>
+    <t>572.9831131190364</t>
+  </si>
+  <si>
+    <t>32.534290304557416</t>
+  </si>
+  <si>
+    <t>39.89761215552263</t>
+  </si>
+  <si>
+    <t>1.791255981687499</t>
+  </si>
+  <si>
+    <t>2.8731889996631668</t>
+  </si>
+  <si>
+    <t>1.0628089876944236</t>
+  </si>
+  <si>
+    <t>0.4589552568351421</t>
+  </si>
+  <si>
+    <t>0.7320554832061781</t>
+  </si>
+  <si>
+    <t>1.4525531306593686</t>
+  </si>
+  <si>
+    <t>0.5007483303467674</t>
+  </si>
+  <si>
+    <t>0.6837150061256506</t>
+  </si>
+  <si>
+    <t>0.6667223919625346</t>
+  </si>
+  <si>
+    <t>0.9946771150104292</t>
+  </si>
+  <si>
+    <t>0.9525406455267272</t>
+  </si>
+  <si>
+    <t>-0.11167865744310965</t>
+  </si>
+  <si>
+    <t>0.532301831731627</t>
+  </si>
+  <si>
+    <t>0.4912083384107137</t>
+  </si>
+  <si>
+    <t>5.664070449571306</t>
+  </si>
+  <si>
+    <t>0.10357914522564642</t>
+  </si>
+  <si>
+    <t>3.813089414989579</t>
+  </si>
+  <si>
+    <t>0.5697396210182328</t>
+  </si>
+  <si>
+    <t>0.1861276114055998</t>
+  </si>
+  <si>
+    <t>11.328140899142614</t>
+  </si>
+  <si>
+    <t>2.769758494666372</t>
+  </si>
+  <si>
+    <t>0.9839994968393977</t>
+  </si>
+  <si>
+    <t>139077.505480233</t>
+  </si>
+  <si>
+    <t>0.2658741561579016</t>
+  </si>
+  <si>
+    <t>1.1916413790063587</t>
+  </si>
+  <si>
+    <t>33.252430173032664</t>
+  </si>
+  <si>
+    <t>4.305672877441645</t>
+  </si>
+  <si>
+    <t>141.0712813781012</t>
+  </si>
+  <si>
+    <t>0.1457962920767277</t>
+  </si>
+  <si>
+    <t>0.03541948318393802</t>
+  </si>
+  <si>
+    <t>3.732741232055689</t>
+  </si>
+  <si>
+    <t>239158.53051793895</t>
+  </si>
+  <si>
+    <t>0.44442695893063117</t>
+  </si>
+  <si>
+    <t>0.604595902366283</t>
+  </si>
+  <si>
+    <t>1.3382653203428032</t>
+  </si>
+  <si>
+    <t>0.6802401681726986</t>
+  </si>
+  <si>
+    <t>22.752127303891044</t>
+  </si>
+  <si>
+    <t>0.02454140448414863</t>
+  </si>
+  <si>
+    <t>2786.386632555165</t>
+  </si>
+  <si>
+    <t>0.22276835885474613</t>
+  </si>
+  <si>
+    <t>4.494727212128211</t>
+  </si>
+  <si>
+    <t>35.31196034537896</t>
+  </si>
+  <si>
+    <t>16668449.423728814</t>
+  </si>
+  <si>
+    <t>534790867.43052447</t>
+  </si>
+  <si>
+    <t>541015.102534323</t>
+  </si>
+  <si>
+    <t>0.05346644575628979</t>
+  </si>
+  <si>
+    <t>2048.2833386632556</t>
+  </si>
+  <si>
+    <t>0.1637578620613412</t>
+  </si>
+  <si>
+    <t>0.39655685878496433</t>
+  </si>
+  <si>
+    <t>13.836531880620292</t>
+  </si>
+  <si>
+    <t>0.02256477885444152</t>
+  </si>
+  <si>
+    <t>6.070772689927588</t>
+  </si>
+  <si>
+    <t>0.014446787818867681</t>
+  </si>
+  <si>
+    <t>16663658.079080952</t>
+  </si>
+  <si>
+    <t>-31.465250076088154</t>
+  </si>
+  <si>
+    <t>35.931272087855476</t>
+  </si>
+  <si>
+    <t>611613975.076851</t>
+  </si>
+  <si>
+    <t>2.181328758955482</t>
+  </si>
+  <si>
+    <t>35.26570280594453</t>
+  </si>
+  <si>
+    <t>3.137544009761257</t>
+  </si>
+  <si>
+    <t>145.50851501216033</t>
+  </si>
+  <si>
+    <t>21.02494880027998</t>
+  </si>
+  <si>
+    <t>2.224926189872966</t>
+  </si>
+  <si>
+    <t>2.2085627730231314</t>
+  </si>
+  <si>
+    <t>-123.51267698686796</t>
+  </si>
+  <si>
+    <t>269.0211919990283</t>
+  </si>
+  <si>
+    <t>14.628313144920915</t>
+  </si>
+  <si>
+    <t>26.57849656117347</t>
+  </si>
+  <si>
+    <t>0.0099480678496397</t>
+  </si>
+  <si>
+    <t>0.25854638185655593</t>
+  </si>
+  <si>
+    <t>701.4661829019278</t>
+  </si>
+  <si>
+    <t>31.48356155266767</t>
+  </si>
+  <si>
+    <t>27.08416767306081</t>
+  </si>
+  <si>
+    <t>0.06487461971500798</t>
+  </si>
+  <si>
+    <t>2.836727235715822</t>
+  </si>
+  <si>
+    <t>1.96528695328053</t>
+  </si>
+  <si>
+    <t>0.18109917813722548</t>
+  </si>
+  <si>
+    <t>1.0349292489008968</t>
+  </si>
+  <si>
+    <t>1.7741414129464381</t>
+  </si>
+  <si>
+    <t>0.8322608037467637</t>
+  </si>
+  <si>
+    <t>0.6068563217773175</t>
+  </si>
+  <si>
+    <t>0.5720216387424092</t>
+  </si>
+  <si>
+    <t>0.9846039297396201</t>
+  </si>
+  <si>
+    <t>0.9193408766018839</t>
+  </si>
+  <si>
+    <t>-0.05441455415111622</t>
+  </si>
+  <si>
+    <t>0.25663692250653486</t>
+  </si>
+  <si>
+    <t>0.48638814941967906</t>
+  </si>
+  <si>
+    <t>5.591573971720844</t>
+  </si>
+  <si>
+    <t>0.07379527783118554</t>
+  </si>
+  <si>
+    <t>4.238560191314501</t>
+  </si>
+  <si>
+    <t>0.22148758301755864</t>
+  </si>
+  <si>
+    <t>0.13122882165059838</t>
+  </si>
+  <si>
+    <t>11.183147943441687</t>
+  </si>
+  <si>
+    <t>2.7763836490938756</t>
+  </si>
+  <si>
+    <t>1.200503547249088</t>
+  </si>
+  <si>
+    <t>143077.51028925503</t>
+  </si>
+  <si>
+    <t>0.2362922367667003</t>
+  </si>
+  <si>
+    <t>1.396396676815745</t>
+  </si>
+  <si>
+    <t>32.63045248944779</t>
+  </si>
+  <si>
+    <t>2.9110993833245127</t>
+  </si>
+  <si>
+    <t>93.71735053536499</t>
+  </si>
+  <si>
+    <t>0.10372307141926021</t>
+  </si>
+  <si>
+    <t>0.037711613806857495</t>
+  </si>
+  <si>
+    <t>3.497252975245331</t>
+  </si>
+  <si>
+    <t>343670.3415577914</t>
+  </si>
+  <si>
+    <t>0.5554603736460547</t>
+  </si>
+  <si>
+    <t>0.7004352765176883</t>
+  </si>
+  <si>
+    <t>0.7645002537243819</t>
+  </si>
+  <si>
+    <t>0.767101146256879</t>
+  </si>
+  <si>
+    <t>25.146278036025766</t>
+  </si>
+  <si>
+    <t>0.029511923296469164</t>
+  </si>
+  <si>
+    <t>5077.71964571288</t>
+  </si>
+  <si>
+    <t>0.20821419796255708</t>
+  </si>
+  <si>
+    <t>5.450805986515106</t>
+  </si>
+  <si>
+    <t>36.40193545741584</t>
+  </si>
+  <si>
+    <t>7495015.682863821</t>
+  </si>
+  <si>
+    <t>238571149.06741297</t>
+  </si>
+  <si>
+    <t>250354.55594453285</t>
+  </si>
+  <si>
+    <t>0.0612544667085605</t>
+  </si>
+  <si>
+    <t>5197.291220732357</t>
+  </si>
+  <si>
+    <t>0.21311728464888496</t>
+  </si>
+  <si>
+    <t>0.45325282598665334</t>
+  </si>
+  <si>
+    <t>16.490748519128115</t>
+  </si>
+  <si>
+    <t>0.029650256054562875</t>
+  </si>
+  <si>
+    <t>5.4312771060799445</t>
+  </si>
+  <si>
+    <t>0.028167078233028952</t>
+  </si>
+  <si>
+    <t>7493755.259630328</t>
+  </si>
+  <si>
+    <t>-12.177929290401467</t>
+  </si>
+  <si>
+    <t>12.03376099946016</t>
+  </si>
+  <si>
+    <t>78470345.508485</t>
+  </si>
+  <si>
+    <t>1.0794920557397851</t>
+  </si>
+  <si>
+    <t>12.679864082454332</t>
+  </si>
+  <si>
+    <t>3.1351310719314</t>
+  </si>
+  <si>
+    <t>52.183798508413</t>
+  </si>
+  <si>
+    <t>7.554201579815505</t>
+  </si>
+  <si>
+    <t>-0.0692641053074522</t>
+  </si>
+  <si>
+    <t>-0.07249681448459061</t>
+  </si>
+  <si>
+    <t>-51.16990027047111</t>
+  </si>
+  <si>
+    <t>103.35369877888411</t>
+  </si>
+  <si>
+    <t>5.252191157458684</t>
+  </si>
+  <si>
+    <t>9.5201653903358</t>
+  </si>
+  <si>
+    <t>-0.001233756137543486</t>
+  </si>
+  <si>
+    <t>0.4903153679430016</t>
+  </si>
+  <si>
+    <t>90.62875154306353</t>
+  </si>
+  <si>
+    <t>12.231376310991946</t>
+  </si>
+  <si>
+    <t>0.6819289216911029</t>
+  </si>
+  <si>
+    <t>0.002441657815017211</t>
+  </si>
+  <si>
+    <t>0.5504761057608607</t>
+  </si>
+  <si>
+    <t>0.5278415410362391</t>
+  </si>
+  <si>
+    <t>0.020993657951885666</t>
+  </si>
+  <si>
+    <t>0.507696457892452</t>
+  </si>
+  <si>
+    <t>1.0477941242669513</t>
+  </si>
+  <si>
+    <t>0.262165828586527</t>
+  </si>
+  <si>
+    <t>0.7494717057090169</t>
+  </si>
+  <si>
+    <t>0.7481660711679793</t>
+  </si>
+  <si>
+    <t>0.9858185484256825</t>
+  </si>
+  <si>
+    <t>0.9278298717059232</t>
+  </si>
+  <si>
+    <t>-0.023954328600698373</t>
+  </si>
+  <si>
+    <t>0.118834577774355</t>
+  </si>
+  <si>
+    <t>0.4904229603178113</t>
+  </si>
+  <si>
+    <t>3.4965292538774295</t>
+  </si>
+  <si>
+    <t>0.24781678273767388</t>
+  </si>
+  <si>
+    <t>2.1329378750407715</t>
+  </si>
+  <si>
+    <t>0.10148077128278142</t>
+  </si>
+  <si>
+    <t>0.2691756816316141</t>
+  </si>
+  <si>
+    <t>6.993058507754858</t>
+  </si>
+  <si>
+    <t>1.5667471752267832</t>
+  </si>
+  <si>
+    <t>0.269579411699275</t>
+  </si>
+  <si>
+    <t>216489.64517883325</t>
+  </si>
+  <si>
+    <t>0.4816684942660853</t>
+  </si>
+  <si>
+    <t>0.28742608257321</t>
+  </si>
+  <si>
+    <t>12.53385401906662</t>
+  </si>
+  <si>
+    <t>6.4394938494670395</t>
+  </si>
+  <si>
+    <t>80.24236899766206</t>
+  </si>
+  <si>
+    <t>0.5623608151175828</t>
+  </si>
+  <si>
+    <t>0.08793550114626754</t>
+  </si>
+  <si>
+    <t>3.028523271433434</t>
+  </si>
+  <si>
+    <t>164975.77077288224</t>
+  </si>
+  <si>
+    <t>0.3566145288951648</t>
+  </si>
+  <si>
+    <t>0.5187248331330438</t>
+  </si>
+  <si>
+    <t>2.045343581715005</t>
+  </si>
+  <si>
+    <t>0.5782038567673431</t>
+  </si>
+  <si>
+    <t>7.2720129639171915</t>
+  </si>
+  <si>
+    <t>0.05119665175774481</t>
+  </si>
+  <si>
+    <t>2670.6039273805113</t>
+  </si>
+  <si>
+    <t>0.4947395197073937</t>
+  </si>
+  <si>
+    <t>2.2444272857223067</t>
+  </si>
+  <si>
+    <t>14.357354575768804</t>
+  </si>
+  <si>
+    <t>68075330.38125232</t>
+  </si>
+  <si>
+    <t>848110160.2160059</t>
+  </si>
+  <si>
+    <t>5928980.09771896</t>
+  </si>
+  <si>
+    <t>0.14652705734634228</t>
+  </si>
+  <si>
+    <t>2409.0452019266395</t>
+  </si>
+  <si>
+    <t>0.44628477249474613</t>
+  </si>
+  <si>
+    <t>0.6780156364893899</t>
+  </si>
+  <si>
+    <t>9.822293158142964</t>
+  </si>
+  <si>
+    <t>0.09861946889961455</t>
+  </si>
+  <si>
+    <t>2.5259366801223524</t>
+  </si>
+  <si>
+    <t>0.006234710636892208</t>
+  </si>
+  <si>
+    <t>68049604.6696861</t>
+  </si>
+  <si>
+    <t>-23.63646383635802</t>
+  </si>
+  <si>
+    <t>32.502869708689076</t>
+  </si>
+  <si>
+    <t>481577225.1338874</t>
+  </si>
+  <si>
+    <t>1.985306168213615</t>
+  </si>
+  <si>
+    <t>28.68030729263449</t>
+  </si>
+  <si>
+    <t>4.54442795132334</t>
+  </si>
+  <si>
+    <t>186.25599936472315</t>
+  </si>
+  <si>
+    <t>17.793484961363493</t>
+  </si>
+  <si>
+    <t>4.287683787553755</t>
+  </si>
+  <si>
+    <t>3.6099951725589463</t>
+  </si>
+  <si>
+    <t>-131.9468470264831</t>
+  </si>
+  <si>
+    <t>318.20284639120626</t>
+  </si>
+  <si>
+    <t>11.94711594504038</t>
+  </si>
+  <si>
+    <t>23.584391790536905</t>
+  </si>
+  <si>
+    <t>0.36744773542387815</t>
+  </si>
+  <si>
+    <t>0.305111670132091</t>
+  </si>
+  <si>
+    <t>537.8393038674932</t>
+  </si>
+  <si>
+    <t>44.94670097561163</t>
+  </si>
+  <si>
+    <t>35.24636899998439</t>
+  </si>
+  <si>
+    <t>1.8051754352492542</t>
+  </si>
+  <si>
+    <t>2.73249609535221</t>
+  </si>
+  <si>
+    <t>0.9628922156873058</t>
+  </si>
+  <si>
+    <t>0.47742155098473593</t>
+  </si>
+  <si>
+    <t>0.6901445010372722</t>
+  </si>
+  <si>
+    <t>1.4029421748673592</t>
+  </si>
+  <si>
+    <t>0.4633880702114807</t>
+  </si>
+  <si>
+    <t>0.6966261685709353</t>
+  </si>
+  <si>
+    <t>0.6820197525295133</t>
+  </si>
+  <si>
+    <t>0.9951684509328825</t>
+  </si>
+  <si>
+    <t>0.9551035309236051</t>
+  </si>
+  <si>
+    <t>-0.12086655604520319</t>
+  </si>
+  <si>
+    <t>0.5517833631836256</t>
+  </si>
+  <si>
+    <t>0.4857164063146773</t>
+  </si>
+  <si>
+    <t>6.671153699044627</t>
+  </si>
+  <si>
+    <t>0.11207709036995334</t>
+  </si>
+  <si>
+    <t>3.70492739146326</t>
+  </si>
+  <si>
+    <t>0.5503423038662576</t>
+  </si>
+  <si>
+    <t>0.2007905124218215</t>
+  </si>
+  <si>
+    <t>13.342307398089257</t>
+  </si>
+  <si>
+    <t>2.7290183724513617</t>
+  </si>
+  <si>
+    <t>0.9238470777598788</t>
+  </si>
+  <si>
+    <t>138494.95493637308</t>
+  </si>
+  <si>
+    <t>0.27306389372708956</t>
+  </si>
+  <si>
+    <t>1.1411970831011535</t>
+  </si>
+  <si>
+    <t>45.7449044312341</t>
+  </si>
+  <si>
+    <t>4.67336989888652</t>
+  </si>
+  <si>
+    <t>211.05431315800402</t>
+  </si>
+  <si>
+    <t>0.1106483386469889</t>
+  </si>
+  <si>
+    <t>0.02432376612872688</t>
+  </si>
+  <si>
+    <t>3.765941227555402</t>
+  </si>
+  <si>
+    <t>222395.70211247142</t>
+  </si>
+  <si>
+    <t>0.4253701724304513</t>
+  </si>
+  <si>
+    <t>0.5861915383709151</t>
+  </si>
+  <si>
+    <t>1.4935448548072292</t>
+  </si>
+  <si>
+    <t>0.6630747553973391</t>
+  </si>
+  <si>
+    <t>30.508859221839224</t>
+  </si>
+  <si>
+    <t>0.01630669005631977</t>
+  </si>
+  <si>
+    <t>2792.221102548903</t>
+  </si>
+  <si>
+    <t>0.23644856486992152</t>
+  </si>
+  <si>
+    <t>4.135889744406914</t>
+  </si>
+  <si>
+    <t>47.97645863324583</t>
+  </si>
+  <si>
+    <t>18054199.241426032</t>
+  </si>
+  <si>
+    <t>794437703.7388432</t>
+  </si>
+  <si>
+    <t>421066.2315463336</t>
+  </si>
+  <si>
+    <t>0.030675861119591665</t>
+  </si>
+  <si>
+    <t>1901.6080108391905</t>
+  </si>
+  <si>
+    <t>0.1610304014598349</t>
+  </si>
+  <si>
+    <t>0.39294145078329346</t>
+  </si>
+  <si>
+    <t>18.830963507324984</t>
+  </si>
+  <si>
+    <t>0.012243550770178786</t>
+  </si>
+  <si>
+    <t>6.048625584434604</t>
+  </si>
+  <si>
+    <t>0.013639440146546885</t>
+  </si>
+  <si>
+    <t>18048823.88939623</t>
+  </si>
+  <si>
+    <t>-8.974111043814647</t>
+  </si>
+  <si>
+    <t>8.831321846818618</t>
+  </si>
+  <si>
+    <t>42035701.46068199</t>
+  </si>
+  <si>
+    <t>1.0059022117946304</t>
+  </si>
+  <si>
+    <t>9.336046390469305</t>
+  </si>
+  <si>
+    <t>3.0597816948472167</t>
+  </si>
+  <si>
+    <t>37.05798848726367</t>
+  </si>
+  <si>
+    <t>5.54551345686056</t>
+  </si>
+  <si>
+    <t>-0.0608504496319161</t>
+  </si>
+  <si>
+    <t>-0.05114878821771163</t>
+  </si>
+  <si>
+    <t>-36.64347824700129</t>
+  </si>
+  <si>
+    <t>73.70146673426495</t>
+  </si>
+  <si>
+    <t>3.8701995271407066</t>
+  </si>
+  <si>
+    <t>6.967883171538404</t>
+  </si>
+  <si>
+    <t>-0.012421989158913226</t>
+  </si>
+  <si>
+    <t>0.4995418130124483</t>
+  </si>
+  <si>
+    <t>48.547693114987695</t>
+  </si>
+  <si>
+    <t>6.24897470300992</t>
+  </si>
+  <si>
+    <t>0.5370586814734856</t>
+  </si>
+  <si>
+    <t>0.002956871995064094</t>
+  </si>
+  <si>
+    <t>0.5300398434138369</t>
+  </si>
+  <si>
+    <t>0.47361912363082737</t>
+  </si>
+  <si>
+    <t>0.056214516821766085</t>
+  </si>
+  <si>
+    <t>0.47286134111722533</t>
+  </si>
+  <si>
+    <t>0.980051328354805</t>
+  </si>
+  <si>
+    <t>0.24260877863120417</t>
+  </si>
+  <si>
+    <t>0.7636955339332382</t>
+  </si>
+  <si>
+    <t>0.7636451076927476</t>
+  </si>
+  <si>
+    <t>0.9721534477134267</t>
+  </si>
+  <si>
+    <t>0.9054529806115323</t>
+  </si>
+  <si>
+    <t>-0.024527289306993588</t>
+  </si>
+  <si>
+    <t>0.16414704190418053</t>
+  </si>
+  <si>
+    <t>0.4721991559143473</t>
+  </si>
+  <si>
+    <t>2.4969719930808383</t>
+  </si>
+  <si>
+    <t>0.2577151311889256</t>
+  </si>
+  <si>
+    <t>1.9868362498672982</t>
+  </si>
+  <si>
+    <t>0.13997331310989042</t>
+  </si>
+  <si>
+    <t>0.28611746787316883</t>
+  </si>
+  <si>
+    <t>4.993943986161677</t>
+  </si>
+  <si>
+    <t>1.510025794634319</t>
+  </si>
+  <si>
+    <t>0.25091474176116607</t>
+  </si>
+  <si>
+    <t>213728.56798226543</t>
+  </si>
+  <si>
+    <t>0.4990324940597074</t>
+  </si>
+  <si>
+    <t>0.25194202105424285</t>
+  </si>
+  <si>
+    <t>6.499161073795521</t>
+  </si>
+  <si>
+    <t>7.250952264653881</t>
+  </si>
+  <si>
+    <t>46.91357178474845</t>
+  </si>
+  <si>
+    <t>1.315737584398471</t>
+  </si>
+  <si>
+    <t>0.18101621614754929</t>
+  </si>
+  <si>
+    <t>3.03994794036574</t>
+  </si>
+  <si>
+    <t>145570.37025229784</t>
+  </si>
+  <si>
+    <t>0.3298736492782025</t>
+  </si>
+  <si>
+    <t>0.4946430034221875</t>
+  </si>
+  <si>
+    <t>2.498666322611616</t>
+  </si>
+  <si>
+    <t>0.5663704301885587</t>
+  </si>
+  <si>
+    <t>3.688432015248111</t>
+  </si>
+  <si>
+    <t>0.10249109337858418</t>
+  </si>
+  <si>
+    <t>151.58753709198814</t>
+  </si>
+  <si>
+    <t>0.4498146501245939</t>
+  </si>
+  <si>
+    <t>2.1227975944139685</t>
+  </si>
+  <si>
+    <t>7.786350148367952</t>
+  </si>
+  <si>
+    <t>1111071125.4065282</t>
+  </si>
+  <si>
+    <t>7189152083.029674</t>
+  </si>
+  <si>
+    <t>201521460.60437274</t>
+  </si>
+  <si>
+    <t>0.548260797889878</t>
+  </si>
+  <si>
+    <t>203.973293768546</t>
+  </si>
+  <si>
+    <t>0.6052619993131929</t>
+  </si>
+  <si>
+    <t>0.8048490882230778</t>
+  </si>
+  <si>
+    <t>6.771264811562814</t>
+  </si>
+  <si>
+    <t>0.41267693509674164</t>
+  </si>
+  <si>
+    <t>2.273964089079546</t>
+  </si>
+  <si>
+    <t>0.0003892362883721145</t>
+  </si>
+  <si>
+    <t>1104470678.3056116</t>
+  </si>
+  <si>
+    <t>-11.22838164003099</t>
+  </si>
+  <si>
+    <t>11.156898789813026</t>
+  </si>
+  <si>
+    <t>66949154.02431025</t>
+  </si>
+  <si>
+    <t>1.0489684138128548</t>
+  </si>
+  <si>
+    <t>11.689204507292466</t>
+  </si>
+  <si>
+    <t>3.130115226780524</t>
+  </si>
+  <si>
+    <t>47.82766177776202</t>
+  </si>
+  <si>
+    <t>6.979652934753727</t>
+  </si>
+  <si>
+    <t>-0.03053440379872714</t>
+  </si>
+  <si>
+    <t>-0.025050154479697467</t>
+  </si>
+  <si>
+    <t>-49.53209366004481</t>
+  </si>
+  <si>
+    <t>97.35975543780683</t>
+  </si>
+  <si>
+    <t>4.852687416294376</t>
+  </si>
+  <si>
+    <t>8.793550412028626</t>
+  </si>
+  <si>
+    <t>-0.0016145632690453945</t>
+  </si>
+  <si>
+    <t>0.4945622179697356</t>
+  </si>
+  <si>
+    <t>77.32559649907353</t>
+  </si>
+  <si>
+    <t>6.249904080510167</t>
+  </si>
+  <si>
+    <t>0.6047099800609804</t>
+  </si>
+  <si>
+    <t>0.000585459690594198</t>
+  </si>
+  <si>
+    <t>0.5329487434290934</t>
+  </si>
+  <si>
+    <t>0.5107715237559515</t>
+  </si>
+  <si>
+    <t>0.021245616872702214</t>
+  </si>
+  <si>
+    <t>0.4995531632178742</t>
+  </si>
+  <si>
+    <t>1.0222647864530452</t>
+  </si>
+  <si>
+    <t>0.25382922172258415</t>
+  </si>
+  <si>
+    <t>0.752078991220227</t>
+  </si>
+  <si>
+    <t>0.7513452544448707</t>
+  </si>
+  <si>
+    <t>0.970156184080641</t>
+  </si>
+  <si>
+    <t>0.9004616951160163</t>
+  </si>
+  <si>
+    <t>-0.022564811878169964</t>
+  </si>
+  <si>
+    <t>0.11477367054932615</t>
+  </si>
+  <si>
+    <t>0.4898707737259975</t>
+  </si>
+  <si>
+    <t>2.49887156621598</t>
+  </si>
+  <si>
+    <t>0.25174773830935704</t>
+  </si>
+  <si>
+    <t>2.074203034715433</t>
+  </si>
+  <si>
+    <t>0.09810770492633641</t>
+  </si>
+  <si>
+    <t>0.27052074478659793</t>
+  </si>
+  <si>
+    <t>4.997743132431962</t>
+  </si>
+  <si>
+    <t>1.5373436110779959</t>
+  </si>
+  <si>
+    <t>0.2609300667962612</t>
+  </si>
+  <si>
+    <t>218430.4182489592</t>
+  </si>
+  <si>
+    <t>0.48954059447707754</t>
+  </si>
+  <si>
+    <t>0.27115339273727335</t>
+  </si>
+  <si>
+    <t>6.517622450947661</t>
+  </si>
+  <si>
+    <t>6.507467170732531</t>
+  </si>
+  <si>
+    <t>42.26932611841842</t>
+  </si>
+  <si>
+    <t>1.1808198289085323</t>
+  </si>
+  <si>
+    <t>0.1844211649136907</t>
+  </si>
+  <si>
+    <t>2.9991081103641046</t>
+  </si>
+  <si>
+    <t>162225.80820220924</t>
+  </si>
+  <si>
+    <t>0.35336931825398943</t>
+  </si>
+  <si>
+    <t>0.5151096711668577</t>
+  </si>
+  <si>
+    <t>2.0793077650182803</t>
+  </si>
+  <si>
+    <t>0.5739186387137499</t>
+  </si>
+  <si>
+    <t>3.7515672346971787</t>
+  </si>
+  <si>
+    <t>0.10724932980363223</t>
+  </si>
+  <si>
+    <t>1607.1884236453202</t>
+  </si>
+  <si>
+    <t>0.49482402205828824</t>
+  </si>
+  <si>
+    <t>2.2374587468756824</t>
+  </si>
+  <si>
+    <t>8.298029556650246</t>
+  </si>
+  <si>
+    <t>114127589.60283251</t>
+  </si>
+  <si>
+    <t>740574113.6748768</t>
+  </si>
+  <si>
+    <t>20641238.64533944</t>
+  </si>
+  <si>
+    <t>0.5413438184181718</t>
+  </si>
+  <si>
+    <t>1611.6496305418718</t>
+  </si>
+  <si>
+    <t>0.4961975463490985</t>
+  </si>
+  <si>
+    <t>0.7202732586004469</t>
+  </si>
+  <si>
+    <t>5.970305293838615</t>
+  </si>
+  <si>
+    <t>0.3905969791600252</t>
+  </si>
+  <si>
+    <t>2.348169806803324</t>
+  </si>
+  <si>
+    <t>0.0037514524173075012</t>
+  </si>
+  <si>
+    <t>114056533.54400699</t>
+  </si>
+  <si>
+    <t>-4.612218241660464</t>
+  </si>
+  <si>
+    <t>4.619366966140351</t>
+  </si>
+  <si>
+    <t>11385301.318534639</t>
+  </si>
+  <si>
+    <t>0.9999999977828555</t>
+  </si>
+  <si>
+    <t>4.827599948261584</t>
+  </si>
+  <si>
+    <t>3.1342809939473235</t>
+  </si>
+  <si>
+    <t>20.73413781951116</t>
+  </si>
+  <si>
+    <t>2.8781982893893896</t>
+  </si>
+  <si>
+    <t>0.0031335777618723302</t>
+  </si>
+  <si>
+    <t>0.0002326199114555047</t>
+  </si>
+  <si>
+    <t>-23.110049222312373</t>
+  </si>
+  <si>
+    <t>43.84418704182353</t>
+  </si>
+  <si>
+    <t>2.0021081557042364</t>
+  </si>
+  <si>
+    <t>3.626302048868487</t>
+  </si>
+  <si>
+    <t>0.001137587112794885</t>
+  </si>
+  <si>
+    <t>0.500000001536807</t>
+  </si>
+  <si>
+    <t>13.150056730318193</t>
+  </si>
+  <si>
+    <t>2.2469255229448803</t>
+  </si>
+  <si>
+    <t>0.49381847164691217</t>
+  </si>
+  <si>
+    <t>2.8063726239727723e-06</t>
+  </si>
+  <si>
+    <t>0.49381850626287493</t>
+  </si>
+  <si>
+    <t>0.506181095693817</t>
+  </si>
+  <si>
+    <t>-0.012362600969632273</t>
+  </si>
+  <si>
+    <t>0.9941235535664666</t>
+  </si>
+  <si>
+    <t>0.24797120586625412</t>
+  </si>
+  <si>
+    <t>0.7469094521530916</t>
+  </si>
+  <si>
+    <t>0.8987637808612365</t>
+  </si>
+  <si>
+    <t>0.831272968102061</t>
+  </si>
+  <si>
+    <t>-0.005876464434116267</t>
+  </si>
+  <si>
+    <t>0.08781789022793297</t>
+  </si>
+  <si>
+    <t>1.500005356930596</t>
+  </si>
+  <si>
+    <t>0.25202899315539995</t>
+  </si>
+  <si>
+    <t>1.9941229616577767</t>
+  </si>
+  <si>
+    <t>0.07343100157413153</t>
+  </si>
+  <si>
+    <t>0.26842392154669575</t>
+  </si>
+  <si>
+    <t>3.000010713861192</t>
+  </si>
+  <si>
+    <t>1.4879418659639598</t>
+  </si>
+  <si>
+    <t>0.24999990048917298</t>
+  </si>
+  <si>
+    <t>228162.6759661067</t>
+  </si>
+  <si>
+    <t>0.5000006270637936</t>
+  </si>
+  <si>
+    <t>0.24999968646810325</t>
+  </si>
+  <si>
+    <t>2.5001364756599025</t>
+  </si>
+  <si>
+    <t>5.453891049193288</t>
+  </si>
+  <si>
+    <t>13.631944120215325</t>
+  </si>
+  <si>
+    <t>3.409377781437779</t>
+  </si>
+  <si>
+    <t>0.6249658810850244</t>
+  </si>
+  <si>
+    <t>2.873372312126191</t>
+  </si>
+  <si>
+    <t>164199.9083004488</t>
+  </si>
+  <si>
+    <t>0.35871701546157936</t>
+  </si>
+  <si>
+    <t>0.5270568530197219</t>
+  </si>
+  <si>
+    <t>1.7847842362129875</t>
+  </si>
+  <si>
+    <t>0.6025874538921095</t>
+  </si>
+  <si>
+    <t>1.506268346697193</t>
+  </si>
+  <si>
+    <t>0.3766672306908388</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>93698824309.5</t>
+  </si>
+  <si>
+    <t>234261021638.25</t>
+  </si>
+  <si>
+    <t>58558274977.3125</t>
+  </si>
+  <si>
+    <t>0.625</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>80518997544.5</t>
-  </si>
-  <si>
-    <t>201013593482.0</t>
-  </si>
-  <si>
-    <t>50395348560.125</t>
-  </si>
-  <si>
-    <t>0.625</t>
-  </si>
-  <si>
-    <t>1.2419497954352022e-11</t>
-  </si>
-  <si>
-    <t>3.109253455399392e-11</t>
-  </si>
-  <si>
-    <t>7.751238804441546e-12</t>
-  </si>
-  <si>
-    <t>0.9999999999999993</t>
-  </si>
-  <si>
-    <t>3.5241235064324063e-06</t>
-  </si>
-  <si>
-    <t>111222.25</t>
-  </si>
-  <si>
-    <t>-1540.2758336283446</t>
-  </si>
-  <si>
-    <t>-767.948713322586</t>
-  </si>
-  <si>
-    <t>890080395783.0013</t>
-  </si>
-  <si>
-    <t>5.394167870836452</t>
-  </si>
-  <si>
-    <t>410.4289360263324</t>
-  </si>
-  <si>
-    <t>2.444483397279076</t>
-  </si>
-  <si>
-    <t>-356.8700411877823</t>
-  </si>
-  <si>
-    <t>235.42914621176868</t>
-  </si>
-  <si>
-    <t>-1219.6362078341858</t>
-  </si>
-  <si>
-    <t>-1285.213106163417</t>
-  </si>
-  <si>
-    <t>-2348.6785880018506</t>
-  </si>
-  <si>
-    <t>1991.8085468140682</t>
-  </si>
-  <si>
-    <t>172.6106420743504</t>
-  </si>
-  <si>
-    <t>1252.348443004888</t>
-  </si>
-  <si>
-    <t>0.5661514411764693</t>
-  </si>
-  <si>
-    <t>0.027140173772449844</t>
-  </si>
-  <si>
-    <t>80864.1432366129</t>
-  </si>
-  <si>
-    <t>2109.4481938053013</t>
-  </si>
-  <si>
-    <t>477184.02171033475</t>
-  </si>
-  <si>
-    <t>5033.211741074467</t>
-  </si>
-  <si>
-    <t>433.1470183038086</t>
-  </si>
-  <si>
-    <t>28.9860571378059</t>
-  </si>
-  <si>
-    <t>0.8739533820121298</t>
-  </si>
-  <si>
-    <t>3.746481088961258</t>
-  </si>
-  <si>
-    <t>3.4350871553080315</t>
-  </si>
-  <si>
-    <t>14.479497576790282</t>
-  </si>
-  <si>
-    <t>0.35915395215081664</t>
-  </si>
-  <si>
-    <t>0.2758164444182932</t>
-  </si>
-  <si>
-    <t>0.9955915549673627</t>
-  </si>
-  <si>
-    <t>0.9571374254911789</t>
-  </si>
-  <si>
-    <t>-0.22602440708613258</t>
-  </si>
-  <si>
-    <t>0.9476214574411512</t>
-  </si>
-  <si>
-    <t>0.27849524118517033</t>
-  </si>
-  <si>
-    <t>44.81499355076389</t>
-  </si>
-  <si>
-    <t>0.0023638103545868417</t>
-  </si>
-  <si>
-    <t>9.469434287356325</t>
-  </si>
-  <si>
-    <t>0.8925545534364545</t>
-  </si>
-  <si>
-    <t>0.006874758758176205</t>
-  </si>
-  <si>
-    <t>89.62998710152775</t>
-  </si>
-  <si>
-    <t>6.3002473096079505</t>
-  </si>
-  <si>
-    <t>115.5332688604036</t>
-  </si>
-  <si>
-    <t>13376.042138643108</t>
-  </si>
-  <si>
-    <t>0.02641128011869122</t>
-  </si>
-  <si>
-    <t>131.57258350298332</t>
-  </si>
-  <si>
-    <t>2268.6897338218705</t>
-  </si>
-  <si>
-    <t>1.4161553779027563</t>
-  </si>
-  <si>
-    <t>3018.058873628436</t>
-  </si>
-  <si>
-    <t>0.0008480504586739011</t>
-  </si>
-  <si>
-    <t>0.0005690322844458802</t>
-  </si>
-  <si>
-    <t>5.947000276986344</t>
-  </si>
-  <si>
-    <t>413794.0861681387</t>
-  </si>
-  <si>
-    <t>0.816512010396653</t>
-  </si>
-  <si>
-    <t>0.8923111893225563</t>
-  </si>
-  <si>
-    <t>0.15818475100490398</t>
-  </si>
-  <si>
-    <t>0.9220709025795292</t>
-  </si>
-  <si>
-    <t>2126.432700749289</t>
-  </si>
-  <si>
-    <t>0.0005171543749730713</t>
-  </si>
-  <si>
-    <t>3545.5637705228196</t>
-  </si>
-  <si>
-    <t>0.024845058550195993</t>
-  </si>
-  <si>
-    <t>123.57160875482404</t>
-  </si>
-  <si>
-    <t>2938.1682748568746</t>
-  </si>
-  <si>
-    <t>4639.307707400478</t>
-  </si>
-  <si>
-    <t>6044876.51719257</t>
-  </si>
-  <si>
-    <t>3.6896608942304945</t>
-  </si>
-  <si>
-    <t>0.00044027073897982637</t>
-  </si>
-  <si>
-    <t>56280.65331763684</t>
-  </si>
-  <si>
-    <t>0.394379065621426</t>
-  </si>
-  <si>
-    <t>0.6522769629582235</t>
-  </si>
-  <si>
-    <t>1981.259471850678</t>
-  </si>
-  <si>
-    <t>0.00027665302188767583</t>
-  </si>
-  <si>
-    <t>7.546090279038857</t>
-  </si>
-  <si>
-    <t>0.2514585466162247</t>
-  </si>
-  <si>
-    <t>4623.492780173469</t>
+    <t>0.06760204081899467</t>
+  </si>
+  <si>
+    <t>0.08290816327197603</t>
+  </si>
+  <si>
+    <t>0.06377551020574931</t>
+  </si>
+  <si>
+    <t>1.9999999999999987</t>
+  </si>
+  <si>
+    <t>4.620015292250617e-06</t>
+  </si>
+  <si>
+    <t>46848438259.25</t>
+  </si>
+  <si>
+    <t>-1512.4290331727532</t>
+  </si>
+  <si>
+    <t>-717.7153240843038</t>
+  </si>
+  <si>
+    <t>1297941537112.3481</t>
+  </si>
+  <si>
+    <t>5.363362832560972</t>
+  </si>
+  <si>
+    <t>447.6096297162819</t>
+  </si>
+  <si>
+    <t>2.252681915797778</t>
+  </si>
+  <si>
+    <t>-366.506427671126</t>
+  </si>
+  <si>
+    <t>246.08014715305603</t>
+  </si>
+  <si>
+    <t>-1189.1034947393139</t>
+  </si>
+  <si>
+    <t>-1265.704487073503</t>
+  </si>
+  <si>
+    <t>-2332.4348911698426</t>
+  </si>
+  <si>
+    <t>1965.9284634987166</t>
+  </si>
+  <si>
+    <t>186.61638019536113</t>
+  </si>
+  <si>
+    <t>1224.3885974136563</t>
+  </si>
+  <si>
+    <t>0.5391265694470674</t>
+  </si>
+  <si>
+    <t>0.027574169775557412</t>
+  </si>
+  <si>
+    <t>85160.31627532974</t>
+  </si>
+  <si>
+    <t>2234.2484407434845</t>
+  </si>
+  <si>
+    <t>526300.5337898724</t>
+  </si>
+  <si>
+    <t>5845.151847579809</t>
+  </si>
+  <si>
+    <t>469.2058111964713</t>
+  </si>
+  <si>
+    <t>24.49027813178929</t>
+  </si>
+  <si>
+    <t>0.9002981883062469</t>
+  </si>
+  <si>
+    <t>3.5145062442186807</t>
+  </si>
+  <si>
+    <t>3.342724833955588</t>
+  </si>
+  <si>
+    <t>11.690278958328346</t>
+  </si>
+  <si>
+    <t>0.364893243872091</t>
+  </si>
+  <si>
+    <t>0.280951310183248</t>
+  </si>
+  <si>
+    <t>0.9962545944421848</t>
+  </si>
+  <si>
+    <t>0.9594680628394449</t>
+  </si>
+  <si>
+    <t>-0.23833462348250417</t>
+  </si>
+  <si>
+    <t>0.9535607849926849</t>
+  </si>
+  <si>
+    <t>0.2837360242842346</t>
+  </si>
+  <si>
+    <t>46.0765289884074</t>
+  </si>
+  <si>
+    <t>0.0024633351414929043</t>
+  </si>
+  <si>
+    <t>9.373386945893824</t>
+  </si>
+  <si>
+    <t>0.9063449716361425</t>
+  </si>
+  <si>
+    <t>0.007393342230223742</t>
+  </si>
+  <si>
+    <t>92.1530579768149</t>
+  </si>
+  <si>
+    <t>6.285735286640517</t>
+  </si>
+  <si>
+    <t>123.4240223320652</t>
+  </si>
+  <si>
+    <t>20682.3929698968</t>
+  </si>
+  <si>
+    <t>0.026838041976523338</t>
+  </si>
+  <si>
+    <t>137.2139856564265</t>
+  </si>
+  <si>
+    <t>2382.2610749949845</t>
+  </si>
+  <si>
+    <t>1.4262288486981842</t>
+  </si>
+  <si>
+    <t>3227.5625801997135</t>
+  </si>
+  <si>
+    <t>0.0008086013812203986</t>
+  </si>
+  <si>
+    <t>0.0005424564873136117</t>
+  </si>
+  <si>
+    <t>5.92756814303262</t>
+  </si>
+  <si>
+    <t>626638.22086314</t>
+  </si>
+  <si>
+    <t>0.8125254143204143</t>
+  </si>
+  <si>
+    <t>0.89002071366087</t>
+  </si>
+  <si>
+    <t>0.16159546721541942</t>
+  </si>
+  <si>
+    <t>0.9201767668030656</t>
+  </si>
+  <si>
+    <t>2222.2297316471672</t>
+  </si>
+  <si>
+    <t>0.0004928710668693847</t>
+  </si>
+  <si>
+    <t>5014.401697758858</t>
+  </si>
+  <si>
+    <t>0.025112816816120487</t>
+  </si>
+  <si>
+    <t>121.71156143697826</t>
+  </si>
+  <si>
+    <t>2953.3147965443845</t>
+  </si>
+  <si>
+    <t>9515.516183798673</t>
+  </si>
+  <si>
+    <t>12813989.454398397</t>
+  </si>
+  <si>
+    <t>7.259513475135325</t>
+  </si>
+  <si>
+    <t>0.00043470216734034175</t>
+  </si>
+  <si>
+    <t>71418.56888944535</t>
+  </si>
+  <si>
+    <t>0.35767406480253083</t>
+  </si>
+  <si>
+    <t>0.6199375278934925</t>
+  </si>
+  <si>
+    <t>1881.9593871709985</t>
+  </si>
+  <si>
+    <t>0.00025723962704246324</t>
+  </si>
+  <si>
+    <t>7.716187995250423</t>
+  </si>
+  <si>
+    <t>0.23062538837003552</t>
+  </si>
+  <si>
+    <t>9496.714975097233</t>
   </si>
 </sst>
 </file>
@@ -4612,7 +4615,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-364.1172669617841</v>
+        <v>-355.9919116646957</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4620,7 +4623,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-32760.99999999929</v>
+        <v>-1125</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4628,7 +4631,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>32763.00000000074</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4668,7 +4671,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>567517</v>
+        <v>865798</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4700,7 +4703,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.791557766180695</v>
+        <v>0.7573971296189453</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4708,7 +4711,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.4542919425953521</v>
+        <v>0.4050011803476377</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4716,7 +4719,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>74.34720228147575</v>
+        <v>77.57996309895869</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4724,7 +4727,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>163.6551197820791</v>
+        <v>191.5549061668586</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4772,7 +4775,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>129.5424810387366</v>
+        <v>145.0831360952051</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4804,7 +4807,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>567517</v>
+        <v>865798</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -9484,7 +9487,7 @@
         <v>622</v>
       </c>
       <c r="B622" t="s">
-        <v>1291</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="623" spans="1:2">
@@ -9492,7 +9495,7 @@
         <v>623</v>
       </c>
       <c r="B623" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="624" spans="1:2">
@@ -9500,7 +9503,7 @@
         <v>624</v>
       </c>
       <c r="B624" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="625" spans="1:2">
@@ -9508,7 +9511,7 @@
         <v>625</v>
       </c>
       <c r="B625" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="626" spans="1:2">
@@ -9516,7 +9519,7 @@
         <v>626</v>
       </c>
       <c r="B626" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="627" spans="1:2">
@@ -9524,7 +9527,7 @@
         <v>627</v>
       </c>
       <c r="B627" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="628" spans="1:2">
@@ -9532,7 +9535,7 @@
         <v>628</v>
       </c>
       <c r="B628" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="629" spans="1:2">
@@ -9540,7 +9543,7 @@
         <v>629</v>
       </c>
       <c r="B629" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="630" spans="1:2">
@@ -9548,7 +9551,7 @@
         <v>630</v>
       </c>
       <c r="B630" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="631" spans="1:2">
@@ -9556,7 +9559,7 @@
         <v>631</v>
       </c>
       <c r="B631" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="632" spans="1:2">
@@ -9564,7 +9567,7 @@
         <v>632</v>
       </c>
       <c r="B632" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="633" spans="1:2">
@@ -9572,7 +9575,7 @@
         <v>633</v>
       </c>
       <c r="B633" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="634" spans="1:2">
@@ -9580,7 +9583,7 @@
         <v>634</v>
       </c>
       <c r="B634" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="635" spans="1:2">
@@ -9588,7 +9591,7 @@
         <v>635</v>
       </c>
       <c r="B635" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="636" spans="1:2">
@@ -9596,7 +9599,7 @@
         <v>636</v>
       </c>
       <c r="B636" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="637" spans="1:2">
@@ -9604,7 +9607,7 @@
         <v>637</v>
       </c>
       <c r="B637" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="638" spans="1:2">
@@ -9612,7 +9615,7 @@
         <v>638</v>
       </c>
       <c r="B638" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="639" spans="1:2">
@@ -9620,7 +9623,7 @@
         <v>639</v>
       </c>
       <c r="B639" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="640" spans="1:2">
@@ -9628,7 +9631,7 @@
         <v>640</v>
       </c>
       <c r="B640" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="641" spans="1:2">
@@ -9636,7 +9639,7 @@
         <v>641</v>
       </c>
       <c r="B641" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="642" spans="1:2">
@@ -9644,7 +9647,7 @@
         <v>642</v>
       </c>
       <c r="B642" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="643" spans="1:2">
@@ -9652,7 +9655,7 @@
         <v>643</v>
       </c>
       <c r="B643" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="644" spans="1:2">
@@ -9660,7 +9663,7 @@
         <v>644</v>
       </c>
       <c r="B644" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="645" spans="1:2">
@@ -9668,7 +9671,7 @@
         <v>645</v>
       </c>
       <c r="B645" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="646" spans="1:2">
@@ -9676,7 +9679,7 @@
         <v>646</v>
       </c>
       <c r="B646" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="647" spans="1:2">
@@ -9684,7 +9687,7 @@
         <v>647</v>
       </c>
       <c r="B647" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="648" spans="1:2">
@@ -9692,7 +9695,7 @@
         <v>648</v>
       </c>
       <c r="B648" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="649" spans="1:2">
@@ -9700,7 +9703,7 @@
         <v>649</v>
       </c>
       <c r="B649" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="650" spans="1:2">
@@ -9708,7 +9711,7 @@
         <v>650</v>
       </c>
       <c r="B650" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="651" spans="1:2">
@@ -9716,7 +9719,7 @@
         <v>651</v>
       </c>
       <c r="B651" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="652" spans="1:2">
@@ -9724,7 +9727,7 @@
         <v>652</v>
       </c>
       <c r="B652" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="653" spans="1:2">
@@ -9732,7 +9735,7 @@
         <v>653</v>
       </c>
       <c r="B653" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="654" spans="1:2">
@@ -9740,7 +9743,7 @@
         <v>654</v>
       </c>
       <c r="B654" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="655" spans="1:2">
@@ -9748,7 +9751,7 @@
         <v>655</v>
       </c>
       <c r="B655" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="656" spans="1:2">
@@ -9756,7 +9759,7 @@
         <v>656</v>
       </c>
       <c r="B656" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="657" spans="1:2">
@@ -9764,7 +9767,7 @@
         <v>657</v>
       </c>
       <c r="B657" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="658" spans="1:2">
@@ -9772,7 +9775,7 @@
         <v>658</v>
       </c>
       <c r="B658" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="659" spans="1:2">
@@ -9780,7 +9783,7 @@
         <v>659</v>
       </c>
       <c r="B659" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="660" spans="1:2">
@@ -9788,7 +9791,7 @@
         <v>660</v>
       </c>
       <c r="B660" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="661" spans="1:2">
@@ -9796,7 +9799,7 @@
         <v>661</v>
       </c>
       <c r="B661" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="662" spans="1:2">
@@ -9804,7 +9807,7 @@
         <v>662</v>
       </c>
       <c r="B662" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="663" spans="1:2">
@@ -9812,7 +9815,7 @@
         <v>663</v>
       </c>
       <c r="B663" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="664" spans="1:2">
@@ -9820,7 +9823,7 @@
         <v>664</v>
       </c>
       <c r="B664" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="665" spans="1:2">
@@ -9828,7 +9831,7 @@
         <v>665</v>
       </c>
       <c r="B665" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="666" spans="1:2">
@@ -9836,7 +9839,7 @@
         <v>666</v>
       </c>
       <c r="B666" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="667" spans="1:2">
@@ -9844,7 +9847,7 @@
         <v>667</v>
       </c>
       <c r="B667" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="668" spans="1:2">
@@ -9852,7 +9855,7 @@
         <v>668</v>
       </c>
       <c r="B668" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="669" spans="1:2">
@@ -9860,7 +9863,7 @@
         <v>669</v>
       </c>
       <c r="B669" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="670" spans="1:2">
@@ -9868,7 +9871,7 @@
         <v>670</v>
       </c>
       <c r="B670" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="671" spans="1:2">
@@ -9876,7 +9879,7 @@
         <v>671</v>
       </c>
       <c r="B671" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="672" spans="1:2">
@@ -9884,7 +9887,7 @@
         <v>672</v>
       </c>
       <c r="B672" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="673" spans="1:2">
@@ -9892,7 +9895,7 @@
         <v>673</v>
       </c>
       <c r="B673" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="674" spans="1:2">
@@ -9900,7 +9903,7 @@
         <v>674</v>
       </c>
       <c r="B674" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="675" spans="1:2">
@@ -9908,7 +9911,7 @@
         <v>675</v>
       </c>
       <c r="B675" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="676" spans="1:2">
@@ -9916,7 +9919,7 @@
         <v>676</v>
       </c>
       <c r="B676" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="677" spans="1:2">
@@ -9924,7 +9927,7 @@
         <v>677</v>
       </c>
       <c r="B677" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="678" spans="1:2">
@@ -9932,7 +9935,7 @@
         <v>678</v>
       </c>
       <c r="B678" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="679" spans="1:2">
@@ -9940,7 +9943,7 @@
         <v>679</v>
       </c>
       <c r="B679" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="680" spans="1:2">
@@ -9948,7 +9951,7 @@
         <v>680</v>
       </c>
       <c r="B680" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="681" spans="1:2">
@@ -9956,7 +9959,7 @@
         <v>681</v>
       </c>
       <c r="B681" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="682" spans="1:2">
@@ -9964,7 +9967,7 @@
         <v>682</v>
       </c>
       <c r="B682" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="683" spans="1:2">
@@ -9972,7 +9975,7 @@
         <v>683</v>
       </c>
       <c r="B683" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="684" spans="1:2">
@@ -9980,7 +9983,7 @@
         <v>684</v>
       </c>
       <c r="B684" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="685" spans="1:2">
@@ -9988,7 +9991,7 @@
         <v>685</v>
       </c>
       <c r="B685" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="686" spans="1:2">
@@ -9996,7 +9999,7 @@
         <v>686</v>
       </c>
       <c r="B686" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="687" spans="1:2">
@@ -10004,7 +10007,7 @@
         <v>687</v>
       </c>
       <c r="B687" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="688" spans="1:2">
@@ -10012,7 +10015,7 @@
         <v>688</v>
       </c>
       <c r="B688" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="689" spans="1:2">
@@ -10020,7 +10023,7 @@
         <v>689</v>
       </c>
       <c r="B689" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="690" spans="1:2">
@@ -10028,7 +10031,7 @@
         <v>690</v>
       </c>
       <c r="B690" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="691" spans="1:2">
@@ -10036,7 +10039,7 @@
         <v>691</v>
       </c>
       <c r="B691" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="692" spans="1:2">
@@ -10044,7 +10047,7 @@
         <v>692</v>
       </c>
       <c r="B692" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="693" spans="1:2">
@@ -10052,7 +10055,7 @@
         <v>693</v>
       </c>
       <c r="B693" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="694" spans="1:2">
@@ -10060,7 +10063,7 @@
         <v>694</v>
       </c>
       <c r="B694" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="695" spans="1:2">
@@ -10068,7 +10071,7 @@
         <v>695</v>
       </c>
       <c r="B695" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="696" spans="1:2">
@@ -10076,7 +10079,7 @@
         <v>696</v>
       </c>
       <c r="B696" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="697" spans="1:2">
@@ -10084,7 +10087,7 @@
         <v>697</v>
       </c>
       <c r="B697" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="698" spans="1:2">
@@ -10092,7 +10095,7 @@
         <v>698</v>
       </c>
       <c r="B698" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="699" spans="1:2">
@@ -10100,7 +10103,7 @@
         <v>699</v>
       </c>
       <c r="B699" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="700" spans="1:2">
@@ -10108,7 +10111,7 @@
         <v>700</v>
       </c>
       <c r="B700" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="701" spans="1:2">
@@ -10116,7 +10119,7 @@
         <v>701</v>
       </c>
       <c r="B701" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="702" spans="1:2">
@@ -10124,7 +10127,7 @@
         <v>702</v>
       </c>
       <c r="B702" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="703" spans="1:2">
@@ -10132,7 +10135,7 @@
         <v>703</v>
       </c>
       <c r="B703" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>